<commit_message>
IN-1180 update caseowners and tasks assignees to include teams
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC02DA7-319F-2E46-B66D-CCF6E676AE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30956EF9-FA02-6C4C-A3D5-503F870C25D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="3340" windowWidth="42220" windowHeight="30440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17940" yWindow="3340" windowWidth="42220" windowHeight="30440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -46,6 +46,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>added col name
 	-Jennifer Mackown</t>
@@ -59,6 +60,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">removed "no", not required
 </t>
@@ -68,6 +70,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">	-Jennifer Mackown</t>
         </r>
@@ -80,6 +83,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">removed "unknown"
 </t>
@@ -89,6 +93,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">	-Jennifer Mackown</t>
         </r>
@@ -101,6 +106,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>removed 'unique_number' - makes more sense as a calculation than a transformation
 	-Jennifer Mackown</t>
@@ -112,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="831">
   <si>
     <t>table_name</t>
   </si>
@@ -2609,6 +2615,30 @@
   </si>
   <si>
     <t>V32</t>
+  </si>
+  <si>
+    <t>LT1</t>
+  </si>
+  <si>
+    <t>LT2</t>
+  </si>
+  <si>
+    <t>LT3</t>
+  </si>
+  <si>
+    <t>LT4</t>
+  </si>
+  <si>
+    <t>LT5</t>
+  </si>
+  <si>
+    <t>LT6</t>
+  </si>
+  <si>
+    <t>LT7</t>
+  </si>
+  <si>
+    <t>LT8</t>
   </si>
 </sst>
 </file>
@@ -31392,7 +31422,7 @@
   </sheetPr>
   <dimension ref="A1:Q998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B75" sqref="A75:XFD75"/>
     </sheetView>
@@ -35435,8 +35465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A433" workbookViewId="0">
+      <selection activeCell="C479" sqref="C479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -41173,41 +41203,101 @@
         <v>2372</v>
       </c>
     </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A478" s="34" t="s">
+        <v>823</v>
+      </c>
+      <c r="B478" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C478" s="34"/>
+      <c r="D478" s="34">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A479" s="34" t="s">
+        <v>824</v>
+      </c>
+      <c r="B479" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C479" s="34"/>
+      <c r="D479" s="34">
+        <v>2443</v>
+      </c>
+    </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A480" s="37"/>
-      <c r="B480" s="37"/>
-      <c r="C480" s="37"/>
-      <c r="D480" s="37"/>
+      <c r="A480" s="34" t="s">
+        <v>825</v>
+      </c>
+      <c r="B480" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C480" s="34"/>
+      <c r="D480" s="34">
+        <v>2444</v>
+      </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A481" s="37"/>
-      <c r="B481" s="37"/>
-      <c r="C481" s="37"/>
-      <c r="D481" s="37"/>
+      <c r="A481" s="34" t="s">
+        <v>826</v>
+      </c>
+      <c r="B481" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C481" s="34"/>
+      <c r="D481" s="34">
+        <v>2523</v>
+      </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A482" s="37"/>
-      <c r="B482" s="37"/>
-      <c r="C482" s="37"/>
-      <c r="D482" s="37"/>
+      <c r="A482" s="34" t="s">
+        <v>827</v>
+      </c>
+      <c r="B482" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C482" s="34"/>
+      <c r="D482" s="34">
+        <v>2524</v>
+      </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A483" s="37"/>
-      <c r="B483" s="37"/>
-      <c r="C483" s="37"/>
-      <c r="D483" s="37"/>
+      <c r="A483" s="34" t="s">
+        <v>828</v>
+      </c>
+      <c r="B483" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C483" s="34"/>
+      <c r="D483" s="34">
+        <v>2525</v>
+      </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A484" s="37"/>
-      <c r="B484" s="37"/>
-      <c r="C484" s="37"/>
-      <c r="D484" s="37"/>
+      <c r="A484" s="34" t="s">
+        <v>829</v>
+      </c>
+      <c r="B484" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C484" s="34"/>
+      <c r="D484" s="34">
+        <v>2572</v>
+      </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A485" s="37"/>
-      <c r="B485" s="37"/>
-      <c r="C485" s="37"/>
-      <c r="D485" s="37"/>
+      <c r="A485" s="34" t="s">
+        <v>830</v>
+      </c>
+      <c r="B485" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C485" s="34"/>
+      <c r="D485" s="34">
+        <v>3945</v>
+      </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A486" s="37"/>

</xml_diff>

<commit_message>
IN-1233 New P2 assignees added
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B571D-FC97-D245-A69E-34913F6AE843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F984460-4961-6C4D-A0B0-D7EF258E47C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6380" yWindow="2060" windowWidth="35840" windowHeight="20480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="844">
   <si>
     <t>table_name</t>
   </si>
@@ -2639,6 +2639,45 @@
   </si>
   <si>
     <t>CASRECMIGRATION_P2</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>C52</t>
+  </si>
+  <si>
+    <t>R62</t>
+  </si>
+  <si>
+    <t>S02</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>S06</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>S36</t>
+  </si>
+  <si>
+    <t>S52</t>
+  </si>
+  <si>
+    <t>S82</t>
+  </si>
+  <si>
+    <t>C94</t>
+  </si>
+  <si>
+    <t>O24</t>
+  </si>
+  <si>
+    <t>R96</t>
   </si>
 </sst>
 </file>
@@ -31422,9 +31461,9 @@
   </sheetPr>
   <dimension ref="A1:Q998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
+      <selection pane="bottomLeft" activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35465,8 +35504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A433" workbookViewId="0">
-      <selection activeCell="C479" sqref="C479"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="D498" sqref="A486:D498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -41300,82 +41339,160 @@
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A486" s="37"/>
-      <c r="B486" s="37"/>
+      <c r="A486" s="37" t="s">
+        <v>831</v>
+      </c>
+      <c r="B486" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C486" s="37"/>
-      <c r="D486" s="37"/>
+      <c r="D486" s="37">
+        <v>8631</v>
+      </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A487" s="37"/>
-      <c r="B487" s="37"/>
+      <c r="A487" s="37" t="s">
+        <v>832</v>
+      </c>
+      <c r="B487" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C487" s="37"/>
-      <c r="D487" s="37"/>
+      <c r="D487" s="37">
+        <v>743</v>
+      </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A488" s="37"/>
-      <c r="B488" s="37"/>
+      <c r="A488" s="37" t="s">
+        <v>841</v>
+      </c>
+      <c r="B488" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C488" s="37"/>
-      <c r="D488" s="37"/>
+      <c r="D488" s="37">
+        <v>1145</v>
+      </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A489" s="37"/>
-      <c r="B489" s="37"/>
+      <c r="A489" s="37" t="s">
+        <v>842</v>
+      </c>
+      <c r="B489" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C489" s="37"/>
-      <c r="D489" s="37"/>
+      <c r="D489" s="37">
+        <v>2639</v>
+      </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A490" s="37"/>
-      <c r="B490" s="37"/>
+      <c r="A490" s="37" t="s">
+        <v>833</v>
+      </c>
+      <c r="B490" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C490" s="37"/>
-      <c r="D490" s="37"/>
+      <c r="D490" s="37">
+        <v>1003</v>
+      </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A491" s="37"/>
-      <c r="B491" s="37"/>
+      <c r="A491" s="37" t="s">
+        <v>843</v>
+      </c>
+      <c r="B491" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C491" s="37"/>
-      <c r="D491" s="37"/>
+      <c r="D491" s="37">
+        <v>1980</v>
+      </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A492" s="37"/>
-      <c r="B492" s="37"/>
+      <c r="A492" s="37" t="s">
+        <v>834</v>
+      </c>
+      <c r="B492" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C492" s="37"/>
-      <c r="D492" s="37"/>
+      <c r="D492" s="37">
+        <v>8764</v>
+      </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A493" s="37"/>
-      <c r="B493" s="37"/>
+      <c r="A493" s="37" t="s">
+        <v>835</v>
+      </c>
+      <c r="B493" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C493" s="37"/>
-      <c r="D493" s="37"/>
+      <c r="D493" s="37">
+        <v>8765</v>
+      </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A494" s="37"/>
-      <c r="B494" s="37"/>
+      <c r="A494" s="37" t="s">
+        <v>836</v>
+      </c>
+      <c r="B494" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C494" s="37"/>
-      <c r="D494" s="37"/>
+      <c r="D494" s="37">
+        <v>8766</v>
+      </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A495" s="37"/>
-      <c r="B495" s="37"/>
+      <c r="A495" s="37" t="s">
+        <v>837</v>
+      </c>
+      <c r="B495" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C495" s="37"/>
-      <c r="D495" s="37"/>
+      <c r="D495" s="37">
+        <v>8664</v>
+      </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A496" s="37"/>
-      <c r="B496" s="37"/>
+      <c r="A496" s="37" t="s">
+        <v>838</v>
+      </c>
+      <c r="B496" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C496" s="37"/>
-      <c r="D496" s="37"/>
+      <c r="D496" s="37">
+        <v>8767</v>
+      </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A497" s="37"/>
-      <c r="B497" s="37"/>
+      <c r="A497" s="37" t="s">
+        <v>839</v>
+      </c>
+      <c r="B497" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C497" s="37"/>
-      <c r="D497" s="37"/>
+      <c r="D497" s="37">
+        <v>8763</v>
+      </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A498" s="37"/>
-      <c r="B498" s="37"/>
+      <c r="A498" s="37" t="s">
+        <v>840</v>
+      </c>
+      <c r="B498" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C498" s="37"/>
-      <c r="D498" s="37"/>
+      <c r="D498" s="37">
+        <v>7123</v>
+      </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A499" s="37"/>

</xml_diff>

<commit_message>
IN-1233 New P2 assignees added (#668)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B571D-FC97-D245-A69E-34913F6AE843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F984460-4961-6C4D-A0B0-D7EF258E47C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6380" yWindow="2060" windowWidth="35840" windowHeight="20480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="844">
   <si>
     <t>table_name</t>
   </si>
@@ -2639,6 +2639,45 @@
   </si>
   <si>
     <t>CASRECMIGRATION_P2</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>C52</t>
+  </si>
+  <si>
+    <t>R62</t>
+  </si>
+  <si>
+    <t>S02</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>S06</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>S36</t>
+  </si>
+  <si>
+    <t>S52</t>
+  </si>
+  <si>
+    <t>S82</t>
+  </si>
+  <si>
+    <t>C94</t>
+  </si>
+  <si>
+    <t>O24</t>
+  </si>
+  <si>
+    <t>R96</t>
   </si>
 </sst>
 </file>
@@ -31422,9 +31461,9 @@
   </sheetPr>
   <dimension ref="A1:Q998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
+      <selection pane="bottomLeft" activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35465,8 +35504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A433" workbookViewId="0">
-      <selection activeCell="C479" sqref="C479"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="D498" sqref="A486:D498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -41300,82 +41339,160 @@
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A486" s="37"/>
-      <c r="B486" s="37"/>
+      <c r="A486" s="37" t="s">
+        <v>831</v>
+      </c>
+      <c r="B486" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C486" s="37"/>
-      <c r="D486" s="37"/>
+      <c r="D486" s="37">
+        <v>8631</v>
+      </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A487" s="37"/>
-      <c r="B487" s="37"/>
+      <c r="A487" s="37" t="s">
+        <v>832</v>
+      </c>
+      <c r="B487" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C487" s="37"/>
-      <c r="D487" s="37"/>
+      <c r="D487" s="37">
+        <v>743</v>
+      </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A488" s="37"/>
-      <c r="B488" s="37"/>
+      <c r="A488" s="37" t="s">
+        <v>841</v>
+      </c>
+      <c r="B488" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C488" s="37"/>
-      <c r="D488" s="37"/>
+      <c r="D488" s="37">
+        <v>1145</v>
+      </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A489" s="37"/>
-      <c r="B489" s="37"/>
+      <c r="A489" s="37" t="s">
+        <v>842</v>
+      </c>
+      <c r="B489" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C489" s="37"/>
-      <c r="D489" s="37"/>
+      <c r="D489" s="37">
+        <v>2639</v>
+      </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A490" s="37"/>
-      <c r="B490" s="37"/>
+      <c r="A490" s="37" t="s">
+        <v>833</v>
+      </c>
+      <c r="B490" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C490" s="37"/>
-      <c r="D490" s="37"/>
+      <c r="D490" s="37">
+        <v>1003</v>
+      </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A491" s="37"/>
-      <c r="B491" s="37"/>
+      <c r="A491" s="37" t="s">
+        <v>843</v>
+      </c>
+      <c r="B491" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C491" s="37"/>
-      <c r="D491" s="37"/>
+      <c r="D491" s="37">
+        <v>1980</v>
+      </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A492" s="37"/>
-      <c r="B492" s="37"/>
+      <c r="A492" s="37" t="s">
+        <v>834</v>
+      </c>
+      <c r="B492" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C492" s="37"/>
-      <c r="D492" s="37"/>
+      <c r="D492" s="37">
+        <v>8764</v>
+      </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A493" s="37"/>
-      <c r="B493" s="37"/>
+      <c r="A493" s="37" t="s">
+        <v>835</v>
+      </c>
+      <c r="B493" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C493" s="37"/>
-      <c r="D493" s="37"/>
+      <c r="D493" s="37">
+        <v>8765</v>
+      </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A494" s="37"/>
-      <c r="B494" s="37"/>
+      <c r="A494" s="37" t="s">
+        <v>836</v>
+      </c>
+      <c r="B494" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C494" s="37"/>
-      <c r="D494" s="37"/>
+      <c r="D494" s="37">
+        <v>8766</v>
+      </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A495" s="37"/>
-      <c r="B495" s="37"/>
+      <c r="A495" s="37" t="s">
+        <v>837</v>
+      </c>
+      <c r="B495" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C495" s="37"/>
-      <c r="D495" s="37"/>
+      <c r="D495" s="37">
+        <v>8664</v>
+      </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A496" s="37"/>
-      <c r="B496" s="37"/>
+      <c r="A496" s="37" t="s">
+        <v>838</v>
+      </c>
+      <c r="B496" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C496" s="37"/>
-      <c r="D496" s="37"/>
+      <c r="D496" s="37">
+        <v>8767</v>
+      </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A497" s="37"/>
-      <c r="B497" s="37"/>
+      <c r="A497" s="37" t="s">
+        <v>839</v>
+      </c>
+      <c r="B497" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C497" s="37"/>
-      <c r="D497" s="37"/>
+      <c r="D497" s="37">
+        <v>8763</v>
+      </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A498" s="37"/>
-      <c r="B498" s="37"/>
+      <c r="A498" s="37" t="s">
+        <v>840</v>
+      </c>
+      <c r="B498" s="37" t="s">
+        <v>331</v>
+      </c>
       <c r="C498" s="37"/>
-      <c r="D498" s="37"/>
+      <c r="D498" s="37">
+        <v>7123</v>
+      </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A499" s="37"/>

</xml_diff>

<commit_message>
IN-1253 make initial P3 changes
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F984460-4961-6C4D-A0B0-D7EF258E47C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E07E4E-7B19-D247-9DDA-901CDF2AD878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="2060" windowWidth="35840" windowHeight="20480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -2638,9 +2638,6 @@
     <t>LT8</t>
   </si>
   <si>
-    <t>CASRECMIGRATION_P2</t>
-  </si>
-  <si>
     <t>C41</t>
   </si>
   <si>
@@ -2678,6 +2675,9 @@
   </si>
   <si>
     <t>R96</t>
+  </si>
+  <si>
+    <t>CASRECMIGRATION_P3</t>
   </si>
 </sst>
 </file>
@@ -31461,9 +31461,9 @@
   </sheetPr>
   <dimension ref="A1:Q998"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M75" sqref="M75"/>
+      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -34000,7 +34000,7 @@
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4" t="s">
-        <v>830</v>
+        <v>843</v>
       </c>
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
@@ -35504,8 +35504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
-      <selection activeCell="D498" sqref="A486:D498"/>
+    <sheetView topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="C491" sqref="C491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -41340,7 +41340,7 @@
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A486" s="37" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B486" s="37" t="s">
         <v>331</v>
@@ -41352,7 +41352,7 @@
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A487" s="37" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B487" s="37" t="s">
         <v>331</v>
@@ -41364,7 +41364,7 @@
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A488" s="37" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B488" s="37" t="s">
         <v>331</v>
@@ -41376,7 +41376,7 @@
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A489" s="37" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B489" s="37" t="s">
         <v>331</v>
@@ -41388,7 +41388,7 @@
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A490" s="37" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B490" s="37" t="s">
         <v>331</v>
@@ -41400,7 +41400,7 @@
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A491" s="37" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B491" s="37" t="s">
         <v>331</v>
@@ -41412,7 +41412,7 @@
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A492" s="37" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B492" s="37" t="s">
         <v>331</v>
@@ -41424,7 +41424,7 @@
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A493" s="37" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B493" s="37" t="s">
         <v>331</v>
@@ -41436,7 +41436,7 @@
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A494" s="37" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B494" s="37" t="s">
         <v>331</v>
@@ -41448,7 +41448,7 @@
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A495" s="37" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B495" s="37" t="s">
         <v>331</v>
@@ -41460,7 +41460,7 @@
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A496" s="37" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B496" s="37" t="s">
         <v>331</v>
@@ -41472,7 +41472,7 @@
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A497" s="37" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B497" s="37" t="s">
         <v>331</v>
@@ -41484,7 +41484,7 @@
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A498" s="37" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B498" s="37" t="s">
         <v>331</v>

</xml_diff>

<commit_message>
In 1253 - initial stab at phase 3 (#684)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F984460-4961-6C4D-A0B0-D7EF258E47C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E07E4E-7B19-D247-9DDA-901CDF2AD878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="2060" windowWidth="35840" windowHeight="20480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -2638,9 +2638,6 @@
     <t>LT8</t>
   </si>
   <si>
-    <t>CASRECMIGRATION_P2</t>
-  </si>
-  <si>
     <t>C41</t>
   </si>
   <si>
@@ -2678,6 +2675,9 @@
   </si>
   <si>
     <t>R96</t>
+  </si>
+  <si>
+    <t>CASRECMIGRATION_P3</t>
   </si>
 </sst>
 </file>
@@ -31461,9 +31461,9 @@
   </sheetPr>
   <dimension ref="A1:Q998"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M75" sqref="M75"/>
+      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -34000,7 +34000,7 @@
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4" t="s">
-        <v>830</v>
+        <v>843</v>
       </c>
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
@@ -35504,8 +35504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
-      <selection activeCell="D498" sqref="A486:D498"/>
+    <sheetView topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="C491" sqref="C491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -41340,7 +41340,7 @@
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A486" s="37" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B486" s="37" t="s">
         <v>331</v>
@@ -41352,7 +41352,7 @@
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A487" s="37" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B487" s="37" t="s">
         <v>331</v>
@@ -41364,7 +41364,7 @@
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A488" s="37" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B488" s="37" t="s">
         <v>331</v>
@@ -41376,7 +41376,7 @@
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A489" s="37" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B489" s="37" t="s">
         <v>331</v>
@@ -41388,7 +41388,7 @@
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A490" s="37" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B490" s="37" t="s">
         <v>331</v>
@@ -41400,7 +41400,7 @@
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A491" s="37" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B491" s="37" t="s">
         <v>331</v>
@@ -41412,7 +41412,7 @@
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A492" s="37" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B492" s="37" t="s">
         <v>331</v>
@@ -41424,7 +41424,7 @@
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A493" s="37" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B493" s="37" t="s">
         <v>331</v>
@@ -41436,7 +41436,7 @@
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A494" s="37" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B494" s="37" t="s">
         <v>331</v>
@@ -41448,7 +41448,7 @@
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A495" s="37" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B495" s="37" t="s">
         <v>331</v>
@@ -41460,7 +41460,7 @@
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A496" s="37" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B496" s="37" t="s">
         <v>331</v>
@@ -41472,7 +41472,7 @@
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A497" s="37" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B497" s="37" t="s">
         <v>331</v>
@@ -41484,7 +41484,7 @@
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A498" s="37" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B498" s="37" t="s">
         <v>331</v>

</xml_diff>

<commit_message>
IN-1255 default to closed cases team
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E07E4E-7B19-D247-9DDA-901CDF2AD878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809A160B-C614-C541-99F1-A78EEBBBB2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="843">
   <si>
     <t>table_name</t>
   </si>
@@ -1162,9 +1162,6 @@
     <t>Client Phone = not null</t>
   </si>
   <si>
-    <t>caseowner_lookup</t>
-  </si>
-  <si>
     <t>R65</t>
   </si>
   <si>
@@ -2494,9 +2491,6 @@
     <t>P02</t>
   </si>
   <si>
-    <t>PFCWorker</t>
-  </si>
-  <si>
     <t>first_word</t>
   </si>
   <si>
@@ -2678,6 +2672,9 @@
   </si>
   <si>
     <t>CASRECMIGRATION_P3</t>
+  </si>
+  <si>
+    <t>Have now set to just a default</t>
   </si>
 </sst>
 </file>
@@ -31461,9 +31458,9 @@
   </sheetPr>
   <dimension ref="A1:Q998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -31781,7 +31778,7 @@
         <v>44</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -31822,7 +31819,7 @@
         <v>44</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -31863,7 +31860,7 @@
         <v>51</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -33215,7 +33212,7 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
@@ -33223,7 +33220,7 @@
         <v>22</v>
       </c>
       <c r="Q52" s="4" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -33956,25 +33953,21 @@
       <c r="G75" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H75" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>782</v>
-      </c>
+      <c r="H75" s="4"/>
+      <c r="J75" s="4"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="4" t="s">
-        <v>338</v>
-      </c>
+      <c r="L75" s="4"/>
       <c r="M75" s="4">
-        <v>2657</v>
+        <v>8730</v>
       </c>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
       <c r="P75" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q75" s="8"/>
+      <c r="Q75" s="8" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
@@ -34000,7 +33993,7 @@
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
@@ -34095,7 +34088,7 @@
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
       <c r="M79" s="4" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="N79" s="4"/>
       <c r="O79" s="4"/>
@@ -35532,7 +35525,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="37" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>331</v>
@@ -35544,7 +35537,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="37" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>331</v>
@@ -35556,7 +35549,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="37" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>331</v>
@@ -35568,7 +35561,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="37" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>331</v>
@@ -35580,7 +35573,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="37" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>331</v>
@@ -35592,7 +35585,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="37" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>331</v>
@@ -35604,7 +35597,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="37" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B8" s="37" t="s">
         <v>331</v>
@@ -35616,7 +35609,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="37" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>331</v>
@@ -35628,7 +35621,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="37" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B10" s="37" t="s">
         <v>331</v>
@@ -35640,7 +35633,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="37" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B11" s="37" t="s">
         <v>331</v>
@@ -35652,7 +35645,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="37" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>331</v>
@@ -35664,7 +35657,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="37" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B13" s="37" t="s">
         <v>331</v>
@@ -35676,7 +35669,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="37" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>331</v>
@@ -35688,7 +35681,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="37" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>331</v>
@@ -35700,7 +35693,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="37" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>331</v>
@@ -35712,7 +35705,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="37" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>331</v>
@@ -35724,7 +35717,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="37" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>331</v>
@@ -35736,7 +35729,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="37" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B19" s="37" t="s">
         <v>331</v>
@@ -35748,7 +35741,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="37" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B20" s="37" t="s">
         <v>331</v>
@@ -35760,7 +35753,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="37" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B21" s="37" t="s">
         <v>331</v>
@@ -35772,7 +35765,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="37" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B22" s="37" t="s">
         <v>331</v>
@@ -35784,7 +35777,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="37" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B23" s="37" t="s">
         <v>331</v>
@@ -35796,7 +35789,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="37" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B24" s="37" t="s">
         <v>331</v>
@@ -35808,7 +35801,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="37" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B25" s="37" t="s">
         <v>331</v>
@@ -35820,7 +35813,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="37" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B26" s="37" t="s">
         <v>331</v>
@@ -35832,7 +35825,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="37" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B27" s="37" t="s">
         <v>331</v>
@@ -35844,7 +35837,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="37" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B28" s="37" t="s">
         <v>331</v>
@@ -35856,7 +35849,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="37" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B29" s="37" t="s">
         <v>331</v>
@@ -35868,7 +35861,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="37" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B30" s="37" t="s">
         <v>331</v>
@@ -35880,7 +35873,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="37" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B31" s="37" t="s">
         <v>331</v>
@@ -35892,7 +35885,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="37" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B32" s="37" t="s">
         <v>331</v>
@@ -35904,7 +35897,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="37" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B33" s="37" t="s">
         <v>331</v>
@@ -35916,7 +35909,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="37" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B34" s="37" t="s">
         <v>331</v>
@@ -35928,7 +35921,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="37" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B35" s="37" t="s">
         <v>331</v>
@@ -35940,7 +35933,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="37" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B36" s="37" t="s">
         <v>331</v>
@@ -35952,7 +35945,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="37" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B37" s="37" t="s">
         <v>331</v>
@@ -35964,7 +35957,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="37" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B38" s="37" t="s">
         <v>331</v>
@@ -35976,7 +35969,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="37" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B39" s="37" t="s">
         <v>331</v>
@@ -35988,7 +35981,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="37" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B40" s="37" t="s">
         <v>331</v>
@@ -36000,7 +35993,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="37" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B41" s="37" t="s">
         <v>331</v>
@@ -36012,7 +36005,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="37" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B42" s="37" t="s">
         <v>331</v>
@@ -36024,7 +36017,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="37" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B43" s="37" t="s">
         <v>331</v>
@@ -36036,7 +36029,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="37" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B44" s="37" t="s">
         <v>331</v>
@@ -36048,7 +36041,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="37" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B45" s="37" t="s">
         <v>331</v>
@@ -36060,7 +36053,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="37" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B46" s="37" t="s">
         <v>331</v>
@@ -36072,7 +36065,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="37" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B47" s="37" t="s">
         <v>331</v>
@@ -36084,7 +36077,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="37" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B48" s="37" t="s">
         <v>331</v>
@@ -36096,7 +36089,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="37" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B49" s="37" t="s">
         <v>331</v>
@@ -36108,7 +36101,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="37" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B50" s="37" t="s">
         <v>331</v>
@@ -36120,7 +36113,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="37" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B51" s="37" t="s">
         <v>331</v>
@@ -36132,7 +36125,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="37" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B52" s="37" t="s">
         <v>331</v>
@@ -36144,7 +36137,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="37" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B53" s="37" t="s">
         <v>331</v>
@@ -36156,7 +36149,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="37" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B54" s="37" t="s">
         <v>331</v>
@@ -36168,7 +36161,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="37" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B55" s="37" t="s">
         <v>331</v>
@@ -36180,7 +36173,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="37" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B56" s="37" t="s">
         <v>331</v>
@@ -36192,7 +36185,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="37" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B57" s="37" t="s">
         <v>331</v>
@@ -36204,7 +36197,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="37" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B58" s="37" t="s">
         <v>331</v>
@@ -36216,7 +36209,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="37" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B59" s="37" t="s">
         <v>331</v>
@@ -36228,7 +36221,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="37" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B60" s="37" t="s">
         <v>331</v>
@@ -36240,7 +36233,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" s="37" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B61" s="37" t="s">
         <v>331</v>
@@ -36252,7 +36245,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="37" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B62" s="37" t="s">
         <v>331</v>
@@ -36264,7 +36257,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="37" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B63" s="37" t="s">
         <v>331</v>
@@ -36276,7 +36269,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="37" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B64" s="37" t="s">
         <v>331</v>
@@ -36288,7 +36281,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="37" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B65" s="37" t="s">
         <v>331</v>
@@ -36300,7 +36293,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="37" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B66" s="37" t="s">
         <v>331</v>
@@ -36312,7 +36305,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="37" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B67" s="37" t="s">
         <v>331</v>
@@ -36324,7 +36317,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="37" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B68" s="37" t="s">
         <v>331</v>
@@ -36336,7 +36329,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="37" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B69" s="37" t="s">
         <v>331</v>
@@ -36348,7 +36341,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="37" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B70" s="37" t="s">
         <v>331</v>
@@ -36360,7 +36353,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="37" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B71" s="37" t="s">
         <v>331</v>
@@ -36372,7 +36365,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="37" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B72" s="37" t="s">
         <v>331</v>
@@ -36384,7 +36377,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" s="37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B73" s="37" t="s">
         <v>331</v>
@@ -36396,7 +36389,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" s="37" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B74" s="37" t="s">
         <v>331</v>
@@ -36408,7 +36401,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="37" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B75" s="37" t="s">
         <v>331</v>
@@ -36420,7 +36413,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" s="37" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B76" s="37" t="s">
         <v>331</v>
@@ -36432,7 +36425,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" s="37" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B77" s="37" t="s">
         <v>331</v>
@@ -36444,7 +36437,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" s="37" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B78" s="37" t="s">
         <v>331</v>
@@ -36456,7 +36449,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" s="37" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B79" s="37" t="s">
         <v>331</v>
@@ -36468,7 +36461,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" s="37" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B80" s="37" t="s">
         <v>331</v>
@@ -36480,7 +36473,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" s="37" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B81" s="37" t="s">
         <v>331</v>
@@ -36492,7 +36485,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B82" s="37" t="s">
         <v>331</v>
@@ -36504,7 +36497,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="37" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B83" s="37" t="s">
         <v>331</v>
@@ -36516,7 +36509,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" s="37" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B84" s="37" t="s">
         <v>331</v>
@@ -36528,7 +36521,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" s="37" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B85" s="37" t="s">
         <v>331</v>
@@ -36540,7 +36533,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="37" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B86" s="37" t="s">
         <v>331</v>
@@ -36552,7 +36545,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="37" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B87" s="37" t="s">
         <v>331</v>
@@ -36564,7 +36557,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="37" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B88" s="37" t="s">
         <v>331</v>
@@ -36576,7 +36569,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" s="37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B89" s="37" t="s">
         <v>331</v>
@@ -36588,7 +36581,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" s="37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B90" s="37" t="s">
         <v>331</v>
@@ -36600,7 +36593,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" s="37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B91" s="37" t="s">
         <v>331</v>
@@ -36612,7 +36605,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" s="37" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B92" s="37" t="s">
         <v>331</v>
@@ -36624,7 +36617,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="37" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B93" s="37" t="s">
         <v>331</v>
@@ -36636,7 +36629,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" s="37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B94" s="37" t="s">
         <v>331</v>
@@ -36648,7 +36641,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" s="37" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B95" s="37" t="s">
         <v>331</v>
@@ -36660,7 +36653,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" s="37" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B96" s="37" t="s">
         <v>331</v>
@@ -36672,7 +36665,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" s="37" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B97" s="37" t="s">
         <v>331</v>
@@ -36684,7 +36677,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" s="37" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B98" s="37" t="s">
         <v>331</v>
@@ -36696,7 +36689,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" s="37" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B99" s="37" t="s">
         <v>331</v>
@@ -36708,7 +36701,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B100" s="37" t="s">
         <v>331</v>
@@ -36720,7 +36713,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" s="37" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B101" s="37" t="s">
         <v>331</v>
@@ -36732,7 +36725,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" s="37" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B102" s="37" t="s">
         <v>331</v>
@@ -36744,7 +36737,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" s="37" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B103" s="37" t="s">
         <v>331</v>
@@ -36756,7 +36749,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" s="37" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B104" s="37" t="s">
         <v>331</v>
@@ -36768,7 +36761,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" s="37" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B105" s="37" t="s">
         <v>331</v>
@@ -36780,7 +36773,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" s="37" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B106" s="37" t="s">
         <v>331</v>
@@ -36792,7 +36785,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" s="37" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B107" s="37" t="s">
         <v>331</v>
@@ -36804,7 +36797,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B108" s="37" t="s">
         <v>331</v>
@@ -36816,7 +36809,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" s="37" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B109" s="37" t="s">
         <v>331</v>
@@ -36828,7 +36821,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" s="37" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B110" s="37" t="s">
         <v>331</v>
@@ -36840,7 +36833,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B111" s="37" t="s">
         <v>331</v>
@@ -36852,7 +36845,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" s="37" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B112" s="37" t="s">
         <v>331</v>
@@ -36864,7 +36857,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" s="37" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B113" s="37" t="s">
         <v>331</v>
@@ -36876,7 +36869,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" s="37" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B114" s="37" t="s">
         <v>331</v>
@@ -36888,7 +36881,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" s="37" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B115" s="37" t="s">
         <v>331</v>
@@ -36900,7 +36893,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" s="37" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B116" s="37" t="s">
         <v>331</v>
@@ -36912,7 +36905,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" s="37" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B117" s="37" t="s">
         <v>331</v>
@@ -36924,7 +36917,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" s="37" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B118" s="37" t="s">
         <v>331</v>
@@ -36936,7 +36929,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" s="37" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B119" s="37" t="s">
         <v>331</v>
@@ -36948,7 +36941,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" s="37" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B120" s="37" t="s">
         <v>331</v>
@@ -36960,7 +36953,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" s="37" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B121" s="37" t="s">
         <v>331</v>
@@ -36972,7 +36965,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" s="37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B122" s="37" t="s">
         <v>331</v>
@@ -36984,7 +36977,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" s="37" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B123" s="37" t="s">
         <v>331</v>
@@ -36996,7 +36989,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" s="37" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B124" s="37" t="s">
         <v>331</v>
@@ -37008,7 +37001,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" s="37" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B125" s="37" t="s">
         <v>331</v>
@@ -37020,7 +37013,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B126" s="37" t="s">
         <v>331</v>
@@ -37032,7 +37025,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A127" s="37" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B127" s="37" t="s">
         <v>331</v>
@@ -37044,7 +37037,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A128" s="37" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B128" s="37" t="s">
         <v>331</v>
@@ -37056,7 +37049,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A129" s="37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B129" s="37" t="s">
         <v>331</v>
@@ -37068,7 +37061,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A130" s="37" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B130" s="37" t="s">
         <v>331</v>
@@ -37080,7 +37073,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A131" s="37" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B131" s="37" t="s">
         <v>331</v>
@@ -37092,7 +37085,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" s="37" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B132" s="37" t="s">
         <v>331</v>
@@ -37104,7 +37097,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A133" s="37" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B133" s="37" t="s">
         <v>331</v>
@@ -37116,7 +37109,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" s="37" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B134" s="37" t="s">
         <v>331</v>
@@ -37128,7 +37121,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A135" s="37" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B135" s="37" t="s">
         <v>331</v>
@@ -37140,7 +37133,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A136" s="37" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B136" s="37" t="s">
         <v>331</v>
@@ -37152,7 +37145,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A137" s="37" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B137" s="37" t="s">
         <v>331</v>
@@ -37164,7 +37157,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A138" s="37" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B138" s="37" t="s">
         <v>331</v>
@@ -37176,7 +37169,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" s="37" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B139" s="37" t="s">
         <v>331</v>
@@ -37188,7 +37181,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" s="37" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B140" s="37" t="s">
         <v>331</v>
@@ -37200,7 +37193,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A141" s="37" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B141" s="37" t="s">
         <v>331</v>
@@ -37212,7 +37205,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A142" s="37" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B142" s="37" t="s">
         <v>331</v>
@@ -37224,7 +37217,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" s="37" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B143" s="37" t="s">
         <v>331</v>
@@ -37236,7 +37229,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A144" s="37" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B144" s="37" t="s">
         <v>331</v>
@@ -37248,7 +37241,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" s="37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B145" s="37" t="s">
         <v>331</v>
@@ -37260,7 +37253,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" s="37" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B146" s="37" t="s">
         <v>331</v>
@@ -37272,7 +37265,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" s="37" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B147" s="37" t="s">
         <v>331</v>
@@ -37284,7 +37277,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" s="37" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B148" s="37" t="s">
         <v>331</v>
@@ -37296,7 +37289,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" s="37" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B149" s="37" t="s">
         <v>331</v>
@@ -37308,7 +37301,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A150" s="37" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B150" s="37" t="s">
         <v>331</v>
@@ -37320,7 +37313,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A151" s="37" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B151" s="37" t="s">
         <v>331</v>
@@ -37332,7 +37325,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A152" s="37" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B152" s="37" t="s">
         <v>331</v>
@@ -37344,7 +37337,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" s="37" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B153" s="37" t="s">
         <v>331</v>
@@ -37356,7 +37349,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A154" s="37" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B154" s="37" t="s">
         <v>331</v>
@@ -37368,7 +37361,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A155" s="37" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B155" s="37" t="s">
         <v>331</v>
@@ -37380,7 +37373,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" s="37" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B156" s="37" t="s">
         <v>331</v>
@@ -37392,7 +37385,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A157" s="37" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B157" s="37" t="s">
         <v>331</v>
@@ -37404,7 +37397,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A158" s="37" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B158" s="37" t="s">
         <v>331</v>
@@ -37416,7 +37409,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A159" s="37" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B159" s="37" t="s">
         <v>331</v>
@@ -37428,7 +37421,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A160" s="37" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B160" s="37" t="s">
         <v>331</v>
@@ -37440,7 +37433,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A161" s="37" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B161" s="37" t="s">
         <v>331</v>
@@ -37452,7 +37445,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" s="37" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B162" s="37" t="s">
         <v>331</v>
@@ -37464,7 +37457,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" s="37" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B163" s="37" t="s">
         <v>331</v>
@@ -37476,7 +37469,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" s="37" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B164" s="37" t="s">
         <v>331</v>
@@ -37488,7 +37481,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" s="37" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B165" s="37" t="s">
         <v>331</v>
@@ -37500,7 +37493,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" s="37" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B166" s="37" t="s">
         <v>331</v>
@@ -37512,7 +37505,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" s="37" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B167" s="37" t="s">
         <v>331</v>
@@ -37524,7 +37517,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A168" s="37" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B168" s="37" t="s">
         <v>331</v>
@@ -37536,7 +37529,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A169" s="37" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B169" s="37" t="s">
         <v>331</v>
@@ -37548,7 +37541,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A170" s="37" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B170" s="37" t="s">
         <v>331</v>
@@ -37560,7 +37553,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A171" s="37" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B171" s="37" t="s">
         <v>331</v>
@@ -37572,7 +37565,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" s="37" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B172" s="37" t="s">
         <v>331</v>
@@ -37584,7 +37577,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" s="37" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B173" s="37" t="s">
         <v>331</v>
@@ -37596,7 +37589,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" s="37" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B174" s="37" t="s">
         <v>331</v>
@@ -37608,7 +37601,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" s="37" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B175" s="37" t="s">
         <v>331</v>
@@ -37620,7 +37613,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" s="37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B176" s="37" t="s">
         <v>331</v>
@@ -37632,7 +37625,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" s="37" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B177" s="37" t="s">
         <v>331</v>
@@ -37644,7 +37637,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" s="37" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B178" s="37" t="s">
         <v>331</v>
@@ -37656,7 +37649,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" s="37" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B179" s="37" t="s">
         <v>331</v>
@@ -37668,7 +37661,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" s="37" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B180" s="37" t="s">
         <v>331</v>
@@ -37680,7 +37673,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B181" s="37" t="s">
         <v>331</v>
@@ -37692,7 +37685,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" s="37" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B182" s="37" t="s">
         <v>331</v>
@@ -37704,7 +37697,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A183" s="37" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B183" s="37" t="s">
         <v>331</v>
@@ -37716,7 +37709,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A184" s="37" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B184" s="37" t="s">
         <v>331</v>
@@ -37728,7 +37721,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" s="37" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B185" s="37" t="s">
         <v>331</v>
@@ -37740,7 +37733,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B186" s="37" t="s">
         <v>331</v>
@@ -37752,7 +37745,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" s="37" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B187" s="37" t="s">
         <v>331</v>
@@ -37764,7 +37757,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A188" s="37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B188" s="37" t="s">
         <v>331</v>
@@ -37776,7 +37769,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" s="37" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B189" s="37" t="s">
         <v>331</v>
@@ -37788,7 +37781,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" s="37" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B190" s="37" t="s">
         <v>331</v>
@@ -37800,7 +37793,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" s="37" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B191" s="37" t="s">
         <v>331</v>
@@ -37812,7 +37805,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" s="37" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B192" s="37" t="s">
         <v>331</v>
@@ -37824,7 +37817,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" s="37" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B193" s="37" t="s">
         <v>331</v>
@@ -37836,7 +37829,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" s="37" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B194" s="37" t="s">
         <v>331</v>
@@ -37848,7 +37841,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B195" s="37" t="s">
         <v>331</v>
@@ -37860,7 +37853,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" s="37" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B196" s="37" t="s">
         <v>331</v>
@@ -37872,7 +37865,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A197" s="37" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B197" s="37" t="s">
         <v>331</v>
@@ -37884,7 +37877,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A198" s="37" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B198" s="37" t="s">
         <v>331</v>
@@ -37896,7 +37889,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" s="37" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B199" s="37" t="s">
         <v>331</v>
@@ -37908,7 +37901,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" s="37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B200" s="37" t="s">
         <v>331</v>
@@ -37920,7 +37913,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" s="37" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B201" s="37" t="s">
         <v>331</v>
@@ -37932,7 +37925,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" s="37" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B202" s="37" t="s">
         <v>331</v>
@@ -37944,7 +37937,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" s="37" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B203" s="37" t="s">
         <v>331</v>
@@ -37956,7 +37949,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" s="37" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B204" s="37" t="s">
         <v>331</v>
@@ -37968,7 +37961,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" s="37" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B205" s="37" t="s">
         <v>331</v>
@@ -37980,7 +37973,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" s="37" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B206" s="37" t="s">
         <v>331</v>
@@ -37992,7 +37985,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" s="37" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B207" s="37" t="s">
         <v>331</v>
@@ -38004,7 +37997,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" s="37" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B208" s="37" t="s">
         <v>331</v>
@@ -38016,7 +38009,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" s="37" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B209" s="37" t="s">
         <v>331</v>
@@ -38028,7 +38021,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" s="37" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B210" s="37" t="s">
         <v>331</v>
@@ -38040,7 +38033,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" s="37" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B211" s="37" t="s">
         <v>331</v>
@@ -38052,7 +38045,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" s="37" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B212" s="37" t="s">
         <v>331</v>
@@ -38064,7 +38057,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" s="37" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B213" s="37" t="s">
         <v>331</v>
@@ -38076,7 +38069,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" s="37" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B214" s="37" t="s">
         <v>331</v>
@@ -38088,7 +38081,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" s="37" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B215" s="37" t="s">
         <v>331</v>
@@ -38100,7 +38093,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" s="37" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B216" s="37" t="s">
         <v>331</v>
@@ -38112,7 +38105,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" s="37" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B217" s="37" t="s">
         <v>331</v>
@@ -38124,7 +38117,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" s="37" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B218" s="37" t="s">
         <v>331</v>
@@ -38136,7 +38129,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A219" s="37" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B219" s="37" t="s">
         <v>331</v>
@@ -38148,7 +38141,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A220" s="37" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B220" s="37" t="s">
         <v>331</v>
@@ -38160,7 +38153,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A221" s="37" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B221" s="37" t="s">
         <v>331</v>
@@ -38172,7 +38165,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A222" s="37" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B222" s="37" t="s">
         <v>331</v>
@@ -38184,7 +38177,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A223" s="37" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B223" s="37" t="s">
         <v>331</v>
@@ -38196,7 +38189,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A224" s="37" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B224" s="37" t="s">
         <v>331</v>
@@ -38208,7 +38201,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A225" s="37" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B225" s="37" t="s">
         <v>331</v>
@@ -38220,7 +38213,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A226" s="37" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B226" s="37" t="s">
         <v>331</v>
@@ -38232,7 +38225,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A227" s="37" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B227" s="37" t="s">
         <v>331</v>
@@ -38244,7 +38237,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A228" s="37" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B228" s="37" t="s">
         <v>331</v>
@@ -38256,7 +38249,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A229" s="37" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B229" s="37" t="s">
         <v>331</v>
@@ -38268,7 +38261,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A230" s="37" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B230" s="37" t="s">
         <v>331</v>
@@ -38280,7 +38273,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A231" s="37" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B231" s="37" t="s">
         <v>331</v>
@@ -38292,7 +38285,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A232" s="37" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B232" s="37" t="s">
         <v>331</v>
@@ -38304,7 +38297,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A233" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B233" s="37" t="s">
         <v>331</v>
@@ -38316,7 +38309,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A234" s="37" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B234" s="37" t="s">
         <v>331</v>
@@ -38328,7 +38321,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A235" s="37" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B235" s="37" t="s">
         <v>331</v>
@@ -38340,7 +38333,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A236" s="37" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B236" s="37" t="s">
         <v>331</v>
@@ -38352,7 +38345,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A237" s="37" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B237" s="37" t="s">
         <v>331</v>
@@ -38364,7 +38357,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A238" s="37" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B238" s="37" t="s">
         <v>331</v>
@@ -38376,7 +38369,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A239" s="37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B239" s="37" t="s">
         <v>331</v>
@@ -38388,7 +38381,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A240" s="37" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B240" s="37" t="s">
         <v>331</v>
@@ -38400,7 +38393,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A241" s="37" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B241" s="37" t="s">
         <v>331</v>
@@ -38412,7 +38405,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A242" s="37" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B242" s="37" t="s">
         <v>331</v>
@@ -38424,7 +38417,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A243" s="37" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B243" s="37" t="s">
         <v>331</v>
@@ -38436,7 +38429,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A244" s="37" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B244" s="37" t="s">
         <v>331</v>
@@ -38448,7 +38441,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A245" s="37" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B245" s="37" t="s">
         <v>331</v>
@@ -38460,7 +38453,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A246" s="37" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B246" s="37" t="s">
         <v>331</v>
@@ -38472,7 +38465,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A247" s="37" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B247" s="37" t="s">
         <v>331</v>
@@ -38484,7 +38477,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B248" s="37" t="s">
         <v>331</v>
@@ -38496,7 +38489,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" s="37" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B249" s="37" t="s">
         <v>331</v>
@@ -38508,7 +38501,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" s="37" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B250" s="37" t="s">
         <v>331</v>
@@ -38520,7 +38513,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" s="37" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B251" s="37" t="s">
         <v>331</v>
@@ -38532,7 +38525,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" s="37" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B252" s="37" t="s">
         <v>331</v>
@@ -38544,7 +38537,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A253" s="37" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B253" s="37" t="s">
         <v>331</v>
@@ -38556,7 +38549,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A254" s="37" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B254" s="37" t="s">
         <v>331</v>
@@ -38568,7 +38561,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" s="37" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B255" s="37" t="s">
         <v>331</v>
@@ -38580,7 +38573,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" s="37" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B256" s="37" t="s">
         <v>331</v>
@@ -38592,7 +38585,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A257" s="37" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B257" s="37" t="s">
         <v>331</v>
@@ -38604,7 +38597,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A258" s="37" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B258" s="37" t="s">
         <v>331</v>
@@ -38616,7 +38609,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A259" s="37" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B259" s="37" t="s">
         <v>331</v>
@@ -38628,7 +38621,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A260" s="37" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B260" s="37" t="s">
         <v>331</v>
@@ -38640,7 +38633,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A261" s="37" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B261" s="37" t="s">
         <v>331</v>
@@ -38652,7 +38645,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A262" s="37" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B262" s="37" t="s">
         <v>331</v>
@@ -38664,7 +38657,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A263" s="37" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B263" s="37" t="s">
         <v>331</v>
@@ -38676,7 +38669,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A264" s="37" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B264" s="37" t="s">
         <v>331</v>
@@ -38688,7 +38681,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A265" s="37" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B265" s="37" t="s">
         <v>331</v>
@@ -38700,7 +38693,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A266" s="37" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B266" s="37" t="s">
         <v>331</v>
@@ -38712,7 +38705,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A267" s="37" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B267" s="37" t="s">
         <v>331</v>
@@ -38724,7 +38717,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A268" s="37" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B268" s="37" t="s">
         <v>331</v>
@@ -38736,7 +38729,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" s="37" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B269" s="37" t="s">
         <v>331</v>
@@ -38748,7 +38741,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" s="37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B270" s="37" t="s">
         <v>331</v>
@@ -38760,7 +38753,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A271" s="37" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B271" s="37" t="s">
         <v>331</v>
@@ -38772,7 +38765,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A272" s="37" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B272" s="37" t="s">
         <v>331</v>
@@ -38784,7 +38777,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" s="37" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B273" s="37" t="s">
         <v>331</v>
@@ -38796,7 +38789,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" s="37" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B274" s="37" t="s">
         <v>331</v>
@@ -38808,7 +38801,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" s="37" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B275" s="37" t="s">
         <v>331</v>
@@ -38820,7 +38813,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" s="37" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B276" s="37" t="s">
         <v>331</v>
@@ -38832,7 +38825,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A277" s="37" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B277" s="37" t="s">
         <v>331</v>
@@ -38844,7 +38837,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" s="37" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B278" s="37" t="s">
         <v>331</v>
@@ -38856,7 +38849,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B279" s="37" t="s">
         <v>331</v>
@@ -38868,7 +38861,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" s="37" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B280" s="37" t="s">
         <v>331</v>
@@ -38880,7 +38873,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" s="37" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B281" s="37" t="s">
         <v>331</v>
@@ -38892,7 +38885,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" s="37" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B282" s="37" t="s">
         <v>331</v>
@@ -38904,7 +38897,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" s="37" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B283" s="37" t="s">
         <v>331</v>
@@ -38916,7 +38909,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" s="37" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B284" s="37" t="s">
         <v>331</v>
@@ -38928,7 +38921,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" s="37" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B285" s="37" t="s">
         <v>331</v>
@@ -38940,7 +38933,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" s="37" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B286" s="37" t="s">
         <v>331</v>
@@ -38952,7 +38945,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" s="37" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B287" s="37" t="s">
         <v>331</v>
@@ -38964,7 +38957,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" s="37" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B288" s="37" t="s">
         <v>331</v>
@@ -38976,7 +38969,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" s="37" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B289" s="37" t="s">
         <v>331</v>
@@ -38988,7 +38981,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" s="37" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B290" s="37" t="s">
         <v>331</v>
@@ -39000,7 +38993,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" s="37" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B291" s="37" t="s">
         <v>331</v>
@@ -39012,7 +39005,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" s="37" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B292" s="37" t="s">
         <v>331</v>
@@ -39024,7 +39017,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" s="37" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B293" s="37" t="s">
         <v>331</v>
@@ -39036,7 +39029,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" s="37" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B294" s="37" t="s">
         <v>331</v>
@@ -39048,7 +39041,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" s="37" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B295" s="37" t="s">
         <v>331</v>
@@ -39060,7 +39053,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" s="37" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B296" s="37" t="s">
         <v>331</v>
@@ -39072,7 +39065,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A297" s="37" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B297" s="37" t="s">
         <v>331</v>
@@ -39084,7 +39077,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A298" s="37" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B298" s="37" t="s">
         <v>331</v>
@@ -39096,7 +39089,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" s="37" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B299" s="37" t="s">
         <v>331</v>
@@ -39108,7 +39101,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" s="37" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B300" s="37" t="s">
         <v>331</v>
@@ -39120,7 +39113,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" s="37" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B301" s="37" t="s">
         <v>331</v>
@@ -39132,7 +39125,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" s="37" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B302" s="37" t="s">
         <v>331</v>
@@ -39144,7 +39137,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A303" s="37" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B303" s="37" t="s">
         <v>331</v>
@@ -39156,7 +39149,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A304" s="37" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B304" s="37" t="s">
         <v>331</v>
@@ -39168,7 +39161,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" s="37" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B305" s="37" t="s">
         <v>331</v>
@@ -39180,7 +39173,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B306" s="37" t="s">
         <v>331</v>
@@ -39192,7 +39185,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" s="37" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B307" s="37" t="s">
         <v>331</v>
@@ -39204,7 +39197,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A308" s="37" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B308" s="37" t="s">
         <v>331</v>
@@ -39216,7 +39209,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A309" s="37" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B309" s="37" t="s">
         <v>331</v>
@@ -39228,7 +39221,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" s="37" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B310" s="37" t="s">
         <v>331</v>
@@ -39240,7 +39233,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" s="37" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B311" s="37" t="s">
         <v>331</v>
@@ -39252,7 +39245,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" s="37" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B312" s="37" t="s">
         <v>331</v>
@@ -39264,7 +39257,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" s="37" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B313" s="37" t="s">
         <v>331</v>
@@ -39276,7 +39269,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" s="37" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B314" s="37" t="s">
         <v>331</v>
@@ -39288,7 +39281,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" s="37" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B315" s="37" t="s">
         <v>331</v>
@@ -39300,7 +39293,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" s="37" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B316" s="37" t="s">
         <v>331</v>
@@ -39312,7 +39305,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" s="37" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B317" s="37" t="s">
         <v>331</v>
@@ -39324,7 +39317,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" s="37" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B318" s="37" t="s">
         <v>331</v>
@@ -39336,7 +39329,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="37" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B319" s="37" t="s">
         <v>331</v>
@@ -39348,7 +39341,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A320" s="37" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B320" s="37" t="s">
         <v>331</v>
@@ -39360,7 +39353,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A321" s="37" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B321" s="37" t="s">
         <v>331</v>
@@ -39372,7 +39365,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" s="37" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B322" s="37" t="s">
         <v>331</v>
@@ -39384,7 +39377,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A323" s="37" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B323" s="37" t="s">
         <v>331</v>
@@ -39396,7 +39389,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A324" s="37" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B324" s="37" t="s">
         <v>331</v>
@@ -39408,7 +39401,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B325" s="37" t="s">
         <v>331</v>
@@ -39420,7 +39413,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" s="37" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B326" s="37" t="s">
         <v>331</v>
@@ -39432,7 +39425,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" s="37" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B327" s="37" t="s">
         <v>331</v>
@@ -39444,7 +39437,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" s="37" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B328" s="37" t="s">
         <v>331</v>
@@ -39456,7 +39449,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" s="37" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B329" s="37" t="s">
         <v>331</v>
@@ -39468,7 +39461,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" s="37" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B330" s="37" t="s">
         <v>331</v>
@@ -39480,7 +39473,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" s="37" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B331" s="37" t="s">
         <v>331</v>
@@ -39492,7 +39485,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" s="37" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B332" s="37" t="s">
         <v>331</v>
@@ -39504,7 +39497,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" s="37" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B333" s="37" t="s">
         <v>331</v>
@@ -39516,7 +39509,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A334" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B334" s="37" t="s">
         <v>331</v>
@@ -39528,7 +39521,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A335" s="37" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B335" s="37" t="s">
         <v>331</v>
@@ -39540,7 +39533,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" s="37" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B336" s="37" t="s">
         <v>331</v>
@@ -39552,7 +39545,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" s="37" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B337" s="37" t="s">
         <v>331</v>
@@ -39564,7 +39557,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A338" s="37" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B338" s="37" t="s">
         <v>331</v>
@@ -39576,7 +39569,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" s="37" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B339" s="37" t="s">
         <v>331</v>
@@ -39588,7 +39581,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" s="37" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B340" s="37" t="s">
         <v>331</v>
@@ -39600,7 +39593,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" s="37" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B341" s="37" t="s">
         <v>331</v>
@@ -39612,7 +39605,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" s="37" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B342" s="37" t="s">
         <v>331</v>
@@ -39624,7 +39617,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" s="37" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B343" s="37" t="s">
         <v>331</v>
@@ -39636,7 +39629,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" s="37" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B344" s="37" t="s">
         <v>331</v>
@@ -39648,7 +39641,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A345" s="37" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B345" s="37" t="s">
         <v>331</v>
@@ -39660,7 +39653,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A346" s="37" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B346" s="37" t="s">
         <v>331</v>
@@ -39672,7 +39665,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" s="37" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B347" s="37" t="s">
         <v>331</v>
@@ -39684,7 +39677,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A348" s="37" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B348" s="37" t="s">
         <v>331</v>
@@ -39696,7 +39689,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A349" s="37" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B349" s="37" t="s">
         <v>331</v>
@@ -39708,7 +39701,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A350" s="37" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B350" s="37" t="s">
         <v>331</v>
@@ -39720,7 +39713,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" s="37" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B351" s="37" t="s">
         <v>331</v>
@@ -39732,7 +39725,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A352" s="37" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B352" s="37" t="s">
         <v>331</v>
@@ -39744,7 +39737,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A353" s="37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B353" s="37" t="s">
         <v>331</v>
@@ -39756,7 +39749,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A354" s="37" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B354" s="37" t="s">
         <v>331</v>
@@ -39768,7 +39761,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A355" s="37" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B355" s="37" t="s">
         <v>331</v>
@@ -39780,7 +39773,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A356" s="37" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B356" s="37" t="s">
         <v>331</v>
@@ -39792,7 +39785,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A357" s="37" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B357" s="37" t="s">
         <v>331</v>
@@ -39804,7 +39797,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A358" s="37" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B358" s="37" t="s">
         <v>331</v>
@@ -39816,7 +39809,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A359" s="37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B359" s="37" t="s">
         <v>331</v>
@@ -39828,7 +39821,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A360" s="37" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B360" s="37" t="s">
         <v>331</v>
@@ -39840,7 +39833,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A361" s="37" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B361" s="37" t="s">
         <v>331</v>
@@ -39852,7 +39845,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A362" s="37" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B362" s="37" t="s">
         <v>331</v>
@@ -39864,7 +39857,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A363" s="37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B363" s="37" t="s">
         <v>331</v>
@@ -39876,7 +39869,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A364" s="37" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B364" s="37" t="s">
         <v>331</v>
@@ -39888,7 +39881,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A365" s="37" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B365" s="37" t="s">
         <v>331</v>
@@ -39900,7 +39893,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A366" s="37" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B366" s="37" t="s">
         <v>331</v>
@@ -39912,7 +39905,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A367" s="37" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B367" s="37" t="s">
         <v>331</v>
@@ -39924,7 +39917,7 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A368" s="37" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B368" s="37" t="s">
         <v>331</v>
@@ -39936,7 +39929,7 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A369" s="37" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B369" s="37" t="s">
         <v>331</v>
@@ -39948,7 +39941,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A370" s="37" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B370" s="37" t="s">
         <v>331</v>
@@ -39960,7 +39953,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A371" s="37" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B371" s="37" t="s">
         <v>331</v>
@@ -39972,7 +39965,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A372" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B372" s="37" t="s">
         <v>331</v>
@@ -39984,7 +39977,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A373" s="37" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B373" s="37" t="s">
         <v>331</v>
@@ -39996,7 +39989,7 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A374" s="37" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B374" s="37" t="s">
         <v>331</v>
@@ -40008,7 +40001,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A375" s="37" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B375" s="37" t="s">
         <v>331</v>
@@ -40020,7 +40013,7 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A376" s="37" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B376" s="37" t="s">
         <v>331</v>
@@ -40032,7 +40025,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A377" s="37" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B377" s="37" t="s">
         <v>331</v>
@@ -40044,7 +40037,7 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A378" s="37" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B378" s="37" t="s">
         <v>331</v>
@@ -40056,7 +40049,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A379" s="37" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B379" s="37" t="s">
         <v>331</v>
@@ -40068,7 +40061,7 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A380" s="37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B380" s="37" t="s">
         <v>331</v>
@@ -40080,7 +40073,7 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A381" s="37" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B381" s="37" t="s">
         <v>331</v>
@@ -40092,7 +40085,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A382" s="37" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B382" s="37" t="s">
         <v>331</v>
@@ -40104,7 +40097,7 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A383" s="37" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B383" s="37" t="s">
         <v>331</v>
@@ -40116,7 +40109,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A384" s="37" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B384" s="37" t="s">
         <v>331</v>
@@ -40128,7 +40121,7 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A385" s="37" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B385" s="37" t="s">
         <v>331</v>
@@ -40140,7 +40133,7 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A386" s="37" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B386" s="37" t="s">
         <v>331</v>
@@ -40152,7 +40145,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A387" s="37" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B387" s="37" t="s">
         <v>331</v>
@@ -40164,7 +40157,7 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A388" s="37" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B388" s="37" t="s">
         <v>331</v>
@@ -40176,7 +40169,7 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A389" s="37" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B389" s="37" t="s">
         <v>331</v>
@@ -40188,7 +40181,7 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A390" s="37" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B390" s="37" t="s">
         <v>331</v>
@@ -40200,7 +40193,7 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A391" s="37" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B391" s="37" t="s">
         <v>331</v>
@@ -40212,7 +40205,7 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A392" s="37" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B392" s="37" t="s">
         <v>331</v>
@@ -40224,7 +40217,7 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A393" s="37" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B393" s="37" t="s">
         <v>331</v>
@@ -40236,7 +40229,7 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A394" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B394" s="37" t="s">
         <v>331</v>
@@ -40248,7 +40241,7 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A395" s="37" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B395" s="37" t="s">
         <v>331</v>
@@ -40260,7 +40253,7 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A396" s="37" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B396" s="37" t="s">
         <v>331</v>
@@ -40272,7 +40265,7 @@
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A397" s="37" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B397" s="37" t="s">
         <v>331</v>
@@ -40284,7 +40277,7 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A398" s="37" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B398" s="37" t="s">
         <v>331</v>
@@ -40296,7 +40289,7 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A399" s="37" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B399" s="37" t="s">
         <v>331</v>
@@ -40308,7 +40301,7 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A400" s="37" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B400" s="37" t="s">
         <v>331</v>
@@ -40320,7 +40313,7 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A401" s="37" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B401" s="37" t="s">
         <v>331</v>
@@ -40332,7 +40325,7 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A402" s="37" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B402" s="37" t="s">
         <v>331</v>
@@ -40344,7 +40337,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A403" s="37" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B403" s="37" t="s">
         <v>331</v>
@@ -40356,7 +40349,7 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A404" s="37" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B404" s="37" t="s">
         <v>331</v>
@@ -40368,7 +40361,7 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A405" s="37" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B405" s="37" t="s">
         <v>331</v>
@@ -40380,7 +40373,7 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A406" s="37" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B406" s="37" t="s">
         <v>331</v>
@@ -40392,7 +40385,7 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A407" s="37" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B407" s="37" t="s">
         <v>331</v>
@@ -40404,7 +40397,7 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A408" s="37" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B408" s="37" t="s">
         <v>331</v>
@@ -40416,7 +40409,7 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A409" s="37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B409" s="37" t="s">
         <v>331</v>
@@ -40428,7 +40421,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A410" s="37" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B410" s="37" t="s">
         <v>331</v>
@@ -40440,7 +40433,7 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A411" s="37" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B411" s="37" t="s">
         <v>331</v>
@@ -40452,7 +40445,7 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A412" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B412" s="37" t="s">
         <v>331</v>
@@ -40464,7 +40457,7 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A413" s="37" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B413" s="37" t="s">
         <v>331</v>
@@ -40476,7 +40469,7 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A414" s="37" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B414" s="37" t="s">
         <v>331</v>
@@ -40488,7 +40481,7 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A415" s="37" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B415" s="37" t="s">
         <v>331</v>
@@ -40500,7 +40493,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A416" s="37" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B416" s="37" t="s">
         <v>331</v>
@@ -40512,7 +40505,7 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A417" s="37" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B417" s="37" t="s">
         <v>331</v>
@@ -40524,7 +40517,7 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A418" s="37" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B418" s="37" t="s">
         <v>331</v>
@@ -40536,7 +40529,7 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A419" s="37" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B419" s="37" t="s">
         <v>331</v>
@@ -40548,7 +40541,7 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A420" s="37" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B420" s="37" t="s">
         <v>331</v>
@@ -40560,7 +40553,7 @@
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A421" s="37" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B421" s="37" t="s">
         <v>331</v>
@@ -40572,7 +40565,7 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A422" s="37" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B422" s="37" t="s">
         <v>331</v>
@@ -40584,7 +40577,7 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A423" s="37" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B423" s="37" t="s">
         <v>331</v>
@@ -40596,7 +40589,7 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A424" s="37" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B424" s="37" t="s">
         <v>331</v>
@@ -40608,7 +40601,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A425" s="37" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B425" s="37" t="s">
         <v>331</v>
@@ -40620,7 +40613,7 @@
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A426" s="37" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B426" s="37" t="s">
         <v>331</v>
@@ -40632,7 +40625,7 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A427" s="37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B427" s="37" t="s">
         <v>331</v>
@@ -40644,7 +40637,7 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A428" s="37" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B428" s="37" t="s">
         <v>331</v>
@@ -40656,7 +40649,7 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A429" s="37" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B429" s="37" t="s">
         <v>331</v>
@@ -40668,7 +40661,7 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A430" s="37" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B430" s="37" t="s">
         <v>331</v>
@@ -40680,7 +40673,7 @@
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A431" s="37" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B431" s="37" t="s">
         <v>331</v>
@@ -40692,7 +40685,7 @@
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A432" s="37" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B432" s="37" t="s">
         <v>331</v>
@@ -40704,7 +40697,7 @@
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A433" s="37" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B433" s="37" t="s">
         <v>331</v>
@@ -40716,7 +40709,7 @@
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A434" s="37" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B434" s="37" t="s">
         <v>331</v>
@@ -40728,7 +40721,7 @@
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A435" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B435" s="37" t="s">
         <v>331</v>
@@ -40740,7 +40733,7 @@
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A436" s="37" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B436" s="37" t="s">
         <v>331</v>
@@ -40752,7 +40745,7 @@
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A437" s="37" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B437" s="37" t="s">
         <v>331</v>
@@ -40764,7 +40757,7 @@
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A438" s="37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B438" s="37" t="s">
         <v>331</v>
@@ -40776,7 +40769,7 @@
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A439" s="37" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B439" s="37" t="s">
         <v>331</v>
@@ -40788,7 +40781,7 @@
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A440" s="37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B440" s="37" t="s">
         <v>331</v>
@@ -40800,7 +40793,7 @@
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A441" s="37" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B441" s="37" t="s">
         <v>331</v>
@@ -40812,7 +40805,7 @@
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A442" s="37" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B442" s="37" t="s">
         <v>331</v>
@@ -40824,7 +40817,7 @@
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A443" s="37" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B443" s="37" t="s">
         <v>331</v>
@@ -40836,7 +40829,7 @@
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A444" s="37" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B444" s="37" t="s">
         <v>331</v>
@@ -40848,7 +40841,7 @@
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A445" s="37" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B445" s="37" t="s">
         <v>331</v>
@@ -40860,7 +40853,7 @@
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A446" s="37" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B446" s="37" t="s">
         <v>331</v>
@@ -40872,7 +40865,7 @@
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A447" s="37" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B447" s="37" t="s">
         <v>331</v>
@@ -40884,7 +40877,7 @@
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A448" s="37" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B448" s="37" t="s">
         <v>331</v>
@@ -40896,7 +40889,7 @@
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A449" s="37" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B449" s="37" t="s">
         <v>331</v>
@@ -40908,7 +40901,7 @@
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A450" s="37" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B450" s="37" t="s">
         <v>331</v>
@@ -40920,7 +40913,7 @@
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A451" s="37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B451" s="37" t="s">
         <v>331</v>
@@ -40932,7 +40925,7 @@
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A452" s="37" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B452" s="37" t="s">
         <v>331</v>
@@ -40944,7 +40937,7 @@
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A453" s="37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B453" s="37" t="s">
         <v>331</v>
@@ -40956,7 +40949,7 @@
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A454" s="37" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B454" s="37" t="s">
         <v>331</v>
@@ -40968,7 +40961,7 @@
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A455" s="37" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B455" s="37" t="s">
         <v>331</v>
@@ -40980,7 +40973,7 @@
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A456" s="37" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B456" s="37" t="s">
         <v>331</v>
@@ -40992,7 +40985,7 @@
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A457" s="37" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B457" s="37" t="s">
         <v>331</v>
@@ -41004,7 +40997,7 @@
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A458" s="37" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B458" s="37" t="s">
         <v>331</v>
@@ -41016,7 +41009,7 @@
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A459" s="37" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B459" s="37" t="s">
         <v>331</v>
@@ -41028,7 +41021,7 @@
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A460" s="37" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B460" s="37" t="s">
         <v>331</v>
@@ -41040,7 +41033,7 @@
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A461" s="37" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B461" s="37" t="s">
         <v>331</v>
@@ -41052,7 +41045,7 @@
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A462" s="37" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B462" s="37" t="s">
         <v>331</v>
@@ -41064,7 +41057,7 @@
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A463" s="37" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B463" s="37" t="s">
         <v>331</v>
@@ -41076,7 +41069,7 @@
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A464" s="37" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B464" s="37" t="s">
         <v>331</v>
@@ -41088,7 +41081,7 @@
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A465" s="37" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B465" s="37" t="s">
         <v>331</v>
@@ -41100,7 +41093,7 @@
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A466" s="37" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B466" s="37" t="s">
         <v>331</v>
@@ -41112,7 +41105,7 @@
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A467" s="37" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B467" s="37" t="s">
         <v>331</v>
@@ -41124,7 +41117,7 @@
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A468" s="37" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B468" s="37" t="s">
         <v>331</v>
@@ -41136,7 +41129,7 @@
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A469" s="37" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B469" s="37" t="s">
         <v>331</v>
@@ -41148,7 +41141,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A470" s="37" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B470" s="37" t="s">
         <v>331</v>
@@ -41160,7 +41153,7 @@
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A471" s="37" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B471" s="37" t="s">
         <v>331</v>
@@ -41172,7 +41165,7 @@
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A472" s="37" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B472" s="37" t="s">
         <v>331</v>
@@ -41184,7 +41177,7 @@
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A473" s="37" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B473" s="37" t="s">
         <v>331</v>
@@ -41196,7 +41189,7 @@
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A474" s="37" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B474" s="37" t="s">
         <v>331</v>
@@ -41208,7 +41201,7 @@
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A475" s="37" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B475" s="37" t="s">
         <v>331</v>
@@ -41220,7 +41213,7 @@
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A476" s="37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B476" s="37" t="s">
         <v>331</v>
@@ -41232,7 +41225,7 @@
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A477" s="37" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B477" s="37" t="s">
         <v>331</v>
@@ -41244,7 +41237,7 @@
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A478" s="34" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B478" s="37" t="s">
         <v>331</v>
@@ -41256,7 +41249,7 @@
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A479" s="34" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B479" s="37" t="s">
         <v>331</v>
@@ -41268,7 +41261,7 @@
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A480" s="34" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B480" s="37" t="s">
         <v>331</v>
@@ -41280,7 +41273,7 @@
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A481" s="34" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B481" s="37" t="s">
         <v>331</v>
@@ -41292,7 +41285,7 @@
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A482" s="34" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B482" s="37" t="s">
         <v>331</v>
@@ -41304,7 +41297,7 @@
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A483" s="34" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B483" s="37" t="s">
         <v>331</v>
@@ -41316,7 +41309,7 @@
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A484" s="34" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B484" s="37" t="s">
         <v>331</v>
@@ -41328,7 +41321,7 @@
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A485" s="34" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B485" s="37" t="s">
         <v>331</v>
@@ -41340,7 +41333,7 @@
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A486" s="37" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B486" s="37" t="s">
         <v>331</v>
@@ -41352,7 +41345,7 @@
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A487" s="37" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B487" s="37" t="s">
         <v>331</v>
@@ -41364,7 +41357,7 @@
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A488" s="37" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B488" s="37" t="s">
         <v>331</v>
@@ -41376,7 +41369,7 @@
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A489" s="37" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B489" s="37" t="s">
         <v>331</v>
@@ -41388,7 +41381,7 @@
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A490" s="37" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B490" s="37" t="s">
         <v>331</v>
@@ -41400,7 +41393,7 @@
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A491" s="37" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B491" s="37" t="s">
         <v>331</v>
@@ -41412,7 +41405,7 @@
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A492" s="37" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B492" s="37" t="s">
         <v>331</v>
@@ -41424,7 +41417,7 @@
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A493" s="37" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B493" s="37" t="s">
         <v>331</v>
@@ -41436,7 +41429,7 @@
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A494" s="37" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B494" s="37" t="s">
         <v>331</v>
@@ -41448,7 +41441,7 @@
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A495" s="37" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B495" s="37" t="s">
         <v>331</v>
@@ -41460,7 +41453,7 @@
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A496" s="37" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B496" s="37" t="s">
         <v>331</v>
@@ -41472,7 +41465,7 @@
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A497" s="37" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B497" s="37" t="s">
         <v>331</v>
@@ -41484,7 +41477,7 @@
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A498" s="37" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B498" s="37" t="s">
         <v>331</v>

</xml_diff>

<commit_message>
IN-1255 default to closed cases team (#690)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james.warren/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E07E4E-7B19-D247-9DDA-901CDF2AD878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809A160B-C614-C541-99F1-A78EEBBBB2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="843">
   <si>
     <t>table_name</t>
   </si>
@@ -1162,9 +1162,6 @@
     <t>Client Phone = not null</t>
   </si>
   <si>
-    <t>caseowner_lookup</t>
-  </si>
-  <si>
     <t>R65</t>
   </si>
   <si>
@@ -2494,9 +2491,6 @@
     <t>P02</t>
   </si>
   <si>
-    <t>PFCWorker</t>
-  </si>
-  <si>
     <t>first_word</t>
   </si>
   <si>
@@ -2678,6 +2672,9 @@
   </si>
   <si>
     <t>CASRECMIGRATION_P3</t>
+  </si>
+  <si>
+    <t>Have now set to just a default</t>
   </si>
 </sst>
 </file>
@@ -31461,9 +31458,9 @@
   </sheetPr>
   <dimension ref="A1:Q998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -31781,7 +31778,7 @@
         <v>44</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -31822,7 +31819,7 @@
         <v>44</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -31863,7 +31860,7 @@
         <v>51</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -33215,7 +33212,7 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
@@ -33223,7 +33220,7 @@
         <v>22</v>
       </c>
       <c r="Q52" s="4" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -33956,25 +33953,21 @@
       <c r="G75" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H75" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>782</v>
-      </c>
+      <c r="H75" s="4"/>
+      <c r="J75" s="4"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="4" t="s">
-        <v>338</v>
-      </c>
+      <c r="L75" s="4"/>
       <c r="M75" s="4">
-        <v>2657</v>
+        <v>8730</v>
       </c>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
       <c r="P75" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q75" s="8"/>
+      <c r="Q75" s="8" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
@@ -34000,7 +33993,7 @@
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
@@ -34095,7 +34088,7 @@
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
       <c r="M79" s="4" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="N79" s="4"/>
       <c r="O79" s="4"/>
@@ -35532,7 +35525,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="37" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>331</v>
@@ -35544,7 +35537,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="37" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>331</v>
@@ -35556,7 +35549,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="37" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>331</v>
@@ -35568,7 +35561,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="37" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>331</v>
@@ -35580,7 +35573,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="37" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>331</v>
@@ -35592,7 +35585,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="37" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>331</v>
@@ -35604,7 +35597,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="37" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B8" s="37" t="s">
         <v>331</v>
@@ -35616,7 +35609,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="37" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>331</v>
@@ -35628,7 +35621,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="37" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B10" s="37" t="s">
         <v>331</v>
@@ -35640,7 +35633,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="37" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B11" s="37" t="s">
         <v>331</v>
@@ -35652,7 +35645,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="37" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>331</v>
@@ -35664,7 +35657,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="37" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B13" s="37" t="s">
         <v>331</v>
@@ -35676,7 +35669,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="37" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>331</v>
@@ -35688,7 +35681,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="37" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>331</v>
@@ -35700,7 +35693,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="37" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>331</v>
@@ -35712,7 +35705,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="37" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>331</v>
@@ -35724,7 +35717,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="37" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>331</v>
@@ -35736,7 +35729,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="37" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B19" s="37" t="s">
         <v>331</v>
@@ -35748,7 +35741,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="37" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B20" s="37" t="s">
         <v>331</v>
@@ -35760,7 +35753,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="37" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B21" s="37" t="s">
         <v>331</v>
@@ -35772,7 +35765,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="37" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B22" s="37" t="s">
         <v>331</v>
@@ -35784,7 +35777,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="37" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B23" s="37" t="s">
         <v>331</v>
@@ -35796,7 +35789,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="37" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B24" s="37" t="s">
         <v>331</v>
@@ -35808,7 +35801,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="37" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B25" s="37" t="s">
         <v>331</v>
@@ -35820,7 +35813,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="37" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B26" s="37" t="s">
         <v>331</v>
@@ -35832,7 +35825,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="37" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B27" s="37" t="s">
         <v>331</v>
@@ -35844,7 +35837,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="37" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B28" s="37" t="s">
         <v>331</v>
@@ -35856,7 +35849,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="37" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B29" s="37" t="s">
         <v>331</v>
@@ -35868,7 +35861,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="37" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B30" s="37" t="s">
         <v>331</v>
@@ -35880,7 +35873,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="37" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B31" s="37" t="s">
         <v>331</v>
@@ -35892,7 +35885,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="37" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B32" s="37" t="s">
         <v>331</v>
@@ -35904,7 +35897,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="37" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B33" s="37" t="s">
         <v>331</v>
@@ -35916,7 +35909,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="37" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B34" s="37" t="s">
         <v>331</v>
@@ -35928,7 +35921,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="37" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B35" s="37" t="s">
         <v>331</v>
@@ -35940,7 +35933,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="37" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B36" s="37" t="s">
         <v>331</v>
@@ -35952,7 +35945,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="37" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B37" s="37" t="s">
         <v>331</v>
@@ -35964,7 +35957,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="37" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B38" s="37" t="s">
         <v>331</v>
@@ -35976,7 +35969,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="37" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B39" s="37" t="s">
         <v>331</v>
@@ -35988,7 +35981,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="37" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B40" s="37" t="s">
         <v>331</v>
@@ -36000,7 +35993,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="37" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B41" s="37" t="s">
         <v>331</v>
@@ -36012,7 +36005,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="37" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B42" s="37" t="s">
         <v>331</v>
@@ -36024,7 +36017,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="37" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B43" s="37" t="s">
         <v>331</v>
@@ -36036,7 +36029,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="37" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B44" s="37" t="s">
         <v>331</v>
@@ -36048,7 +36041,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="37" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B45" s="37" t="s">
         <v>331</v>
@@ -36060,7 +36053,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="37" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B46" s="37" t="s">
         <v>331</v>
@@ -36072,7 +36065,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="37" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B47" s="37" t="s">
         <v>331</v>
@@ -36084,7 +36077,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="37" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B48" s="37" t="s">
         <v>331</v>
@@ -36096,7 +36089,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="37" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B49" s="37" t="s">
         <v>331</v>
@@ -36108,7 +36101,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="37" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B50" s="37" t="s">
         <v>331</v>
@@ -36120,7 +36113,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="37" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B51" s="37" t="s">
         <v>331</v>
@@ -36132,7 +36125,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="37" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B52" s="37" t="s">
         <v>331</v>
@@ -36144,7 +36137,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="37" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B53" s="37" t="s">
         <v>331</v>
@@ -36156,7 +36149,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="37" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B54" s="37" t="s">
         <v>331</v>
@@ -36168,7 +36161,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="37" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B55" s="37" t="s">
         <v>331</v>
@@ -36180,7 +36173,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="37" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B56" s="37" t="s">
         <v>331</v>
@@ -36192,7 +36185,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="37" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B57" s="37" t="s">
         <v>331</v>
@@ -36204,7 +36197,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="37" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B58" s="37" t="s">
         <v>331</v>
@@ -36216,7 +36209,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="37" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B59" s="37" t="s">
         <v>331</v>
@@ -36228,7 +36221,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="37" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B60" s="37" t="s">
         <v>331</v>
@@ -36240,7 +36233,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" s="37" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B61" s="37" t="s">
         <v>331</v>
@@ -36252,7 +36245,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="37" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B62" s="37" t="s">
         <v>331</v>
@@ -36264,7 +36257,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="37" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B63" s="37" t="s">
         <v>331</v>
@@ -36276,7 +36269,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="37" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B64" s="37" t="s">
         <v>331</v>
@@ -36288,7 +36281,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="37" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B65" s="37" t="s">
         <v>331</v>
@@ -36300,7 +36293,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="37" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B66" s="37" t="s">
         <v>331</v>
@@ -36312,7 +36305,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="37" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B67" s="37" t="s">
         <v>331</v>
@@ -36324,7 +36317,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="37" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B68" s="37" t="s">
         <v>331</v>
@@ -36336,7 +36329,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="37" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B69" s="37" t="s">
         <v>331</v>
@@ -36348,7 +36341,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="37" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B70" s="37" t="s">
         <v>331</v>
@@ -36360,7 +36353,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="37" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B71" s="37" t="s">
         <v>331</v>
@@ -36372,7 +36365,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="37" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B72" s="37" t="s">
         <v>331</v>
@@ -36384,7 +36377,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" s="37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B73" s="37" t="s">
         <v>331</v>
@@ -36396,7 +36389,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" s="37" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B74" s="37" t="s">
         <v>331</v>
@@ -36408,7 +36401,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="37" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B75" s="37" t="s">
         <v>331</v>
@@ -36420,7 +36413,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" s="37" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B76" s="37" t="s">
         <v>331</v>
@@ -36432,7 +36425,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" s="37" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B77" s="37" t="s">
         <v>331</v>
@@ -36444,7 +36437,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" s="37" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B78" s="37" t="s">
         <v>331</v>
@@ -36456,7 +36449,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" s="37" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B79" s="37" t="s">
         <v>331</v>
@@ -36468,7 +36461,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" s="37" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B80" s="37" t="s">
         <v>331</v>
@@ -36480,7 +36473,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" s="37" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B81" s="37" t="s">
         <v>331</v>
@@ -36492,7 +36485,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B82" s="37" t="s">
         <v>331</v>
@@ -36504,7 +36497,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="37" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B83" s="37" t="s">
         <v>331</v>
@@ -36516,7 +36509,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" s="37" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B84" s="37" t="s">
         <v>331</v>
@@ -36528,7 +36521,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" s="37" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B85" s="37" t="s">
         <v>331</v>
@@ -36540,7 +36533,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="37" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B86" s="37" t="s">
         <v>331</v>
@@ -36552,7 +36545,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="37" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B87" s="37" t="s">
         <v>331</v>
@@ -36564,7 +36557,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="37" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B88" s="37" t="s">
         <v>331</v>
@@ -36576,7 +36569,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" s="37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B89" s="37" t="s">
         <v>331</v>
@@ -36588,7 +36581,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" s="37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B90" s="37" t="s">
         <v>331</v>
@@ -36600,7 +36593,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" s="37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B91" s="37" t="s">
         <v>331</v>
@@ -36612,7 +36605,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" s="37" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B92" s="37" t="s">
         <v>331</v>
@@ -36624,7 +36617,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="37" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B93" s="37" t="s">
         <v>331</v>
@@ -36636,7 +36629,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" s="37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B94" s="37" t="s">
         <v>331</v>
@@ -36648,7 +36641,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" s="37" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B95" s="37" t="s">
         <v>331</v>
@@ -36660,7 +36653,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" s="37" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B96" s="37" t="s">
         <v>331</v>
@@ -36672,7 +36665,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" s="37" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B97" s="37" t="s">
         <v>331</v>
@@ -36684,7 +36677,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" s="37" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B98" s="37" t="s">
         <v>331</v>
@@ -36696,7 +36689,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" s="37" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B99" s="37" t="s">
         <v>331</v>
@@ -36708,7 +36701,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B100" s="37" t="s">
         <v>331</v>
@@ -36720,7 +36713,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" s="37" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B101" s="37" t="s">
         <v>331</v>
@@ -36732,7 +36725,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" s="37" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B102" s="37" t="s">
         <v>331</v>
@@ -36744,7 +36737,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" s="37" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B103" s="37" t="s">
         <v>331</v>
@@ -36756,7 +36749,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" s="37" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B104" s="37" t="s">
         <v>331</v>
@@ -36768,7 +36761,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" s="37" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B105" s="37" t="s">
         <v>331</v>
@@ -36780,7 +36773,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" s="37" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B106" s="37" t="s">
         <v>331</v>
@@ -36792,7 +36785,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" s="37" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B107" s="37" t="s">
         <v>331</v>
@@ -36804,7 +36797,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A108" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B108" s="37" t="s">
         <v>331</v>
@@ -36816,7 +36809,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A109" s="37" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B109" s="37" t="s">
         <v>331</v>
@@ -36828,7 +36821,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" s="37" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B110" s="37" t="s">
         <v>331</v>
@@ -36840,7 +36833,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B111" s="37" t="s">
         <v>331</v>
@@ -36852,7 +36845,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" s="37" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B112" s="37" t="s">
         <v>331</v>
@@ -36864,7 +36857,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" s="37" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B113" s="37" t="s">
         <v>331</v>
@@ -36876,7 +36869,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" s="37" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B114" s="37" t="s">
         <v>331</v>
@@ -36888,7 +36881,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" s="37" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B115" s="37" t="s">
         <v>331</v>
@@ -36900,7 +36893,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A116" s="37" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B116" s="37" t="s">
         <v>331</v>
@@ -36912,7 +36905,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" s="37" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B117" s="37" t="s">
         <v>331</v>
@@ -36924,7 +36917,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" s="37" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B118" s="37" t="s">
         <v>331</v>
@@ -36936,7 +36929,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" s="37" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B119" s="37" t="s">
         <v>331</v>
@@ -36948,7 +36941,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" s="37" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B120" s="37" t="s">
         <v>331</v>
@@ -36960,7 +36953,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" s="37" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B121" s="37" t="s">
         <v>331</v>
@@ -36972,7 +36965,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A122" s="37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B122" s="37" t="s">
         <v>331</v>
@@ -36984,7 +36977,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" s="37" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B123" s="37" t="s">
         <v>331</v>
@@ -36996,7 +36989,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" s="37" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B124" s="37" t="s">
         <v>331</v>
@@ -37008,7 +37001,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A125" s="37" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B125" s="37" t="s">
         <v>331</v>
@@ -37020,7 +37013,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B126" s="37" t="s">
         <v>331</v>
@@ -37032,7 +37025,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A127" s="37" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B127" s="37" t="s">
         <v>331</v>
@@ -37044,7 +37037,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A128" s="37" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B128" s="37" t="s">
         <v>331</v>
@@ -37056,7 +37049,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A129" s="37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B129" s="37" t="s">
         <v>331</v>
@@ -37068,7 +37061,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A130" s="37" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B130" s="37" t="s">
         <v>331</v>
@@ -37080,7 +37073,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A131" s="37" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B131" s="37" t="s">
         <v>331</v>
@@ -37092,7 +37085,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" s="37" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B132" s="37" t="s">
         <v>331</v>
@@ -37104,7 +37097,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A133" s="37" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B133" s="37" t="s">
         <v>331</v>
@@ -37116,7 +37109,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" s="37" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B134" s="37" t="s">
         <v>331</v>
@@ -37128,7 +37121,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A135" s="37" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B135" s="37" t="s">
         <v>331</v>
@@ -37140,7 +37133,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A136" s="37" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B136" s="37" t="s">
         <v>331</v>
@@ -37152,7 +37145,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A137" s="37" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B137" s="37" t="s">
         <v>331</v>
@@ -37164,7 +37157,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A138" s="37" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B138" s="37" t="s">
         <v>331</v>
@@ -37176,7 +37169,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" s="37" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B139" s="37" t="s">
         <v>331</v>
@@ -37188,7 +37181,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" s="37" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B140" s="37" t="s">
         <v>331</v>
@@ -37200,7 +37193,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A141" s="37" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B141" s="37" t="s">
         <v>331</v>
@@ -37212,7 +37205,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A142" s="37" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B142" s="37" t="s">
         <v>331</v>
@@ -37224,7 +37217,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" s="37" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B143" s="37" t="s">
         <v>331</v>
@@ -37236,7 +37229,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A144" s="37" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B144" s="37" t="s">
         <v>331</v>
@@ -37248,7 +37241,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A145" s="37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B145" s="37" t="s">
         <v>331</v>
@@ -37260,7 +37253,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" s="37" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B146" s="37" t="s">
         <v>331</v>
@@ -37272,7 +37265,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" s="37" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B147" s="37" t="s">
         <v>331</v>
@@ -37284,7 +37277,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A148" s="37" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B148" s="37" t="s">
         <v>331</v>
@@ -37296,7 +37289,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A149" s="37" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B149" s="37" t="s">
         <v>331</v>
@@ -37308,7 +37301,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A150" s="37" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B150" s="37" t="s">
         <v>331</v>
@@ -37320,7 +37313,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A151" s="37" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B151" s="37" t="s">
         <v>331</v>
@@ -37332,7 +37325,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A152" s="37" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B152" s="37" t="s">
         <v>331</v>
@@ -37344,7 +37337,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" s="37" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B153" s="37" t="s">
         <v>331</v>
@@ -37356,7 +37349,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A154" s="37" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B154" s="37" t="s">
         <v>331</v>
@@ -37368,7 +37361,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A155" s="37" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B155" s="37" t="s">
         <v>331</v>
@@ -37380,7 +37373,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" s="37" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B156" s="37" t="s">
         <v>331</v>
@@ -37392,7 +37385,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A157" s="37" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B157" s="37" t="s">
         <v>331</v>
@@ -37404,7 +37397,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A158" s="37" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B158" s="37" t="s">
         <v>331</v>
@@ -37416,7 +37409,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A159" s="37" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B159" s="37" t="s">
         <v>331</v>
@@ -37428,7 +37421,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A160" s="37" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B160" s="37" t="s">
         <v>331</v>
@@ -37440,7 +37433,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A161" s="37" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B161" s="37" t="s">
         <v>331</v>
@@ -37452,7 +37445,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" s="37" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B162" s="37" t="s">
         <v>331</v>
@@ -37464,7 +37457,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" s="37" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B163" s="37" t="s">
         <v>331</v>
@@ -37476,7 +37469,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" s="37" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B164" s="37" t="s">
         <v>331</v>
@@ -37488,7 +37481,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" s="37" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B165" s="37" t="s">
         <v>331</v>
@@ -37500,7 +37493,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" s="37" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B166" s="37" t="s">
         <v>331</v>
@@ -37512,7 +37505,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" s="37" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B167" s="37" t="s">
         <v>331</v>
@@ -37524,7 +37517,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A168" s="37" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B168" s="37" t="s">
         <v>331</v>
@@ -37536,7 +37529,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A169" s="37" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B169" s="37" t="s">
         <v>331</v>
@@ -37548,7 +37541,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A170" s="37" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B170" s="37" t="s">
         <v>331</v>
@@ -37560,7 +37553,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A171" s="37" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B171" s="37" t="s">
         <v>331</v>
@@ -37572,7 +37565,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" s="37" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B172" s="37" t="s">
         <v>331</v>
@@ -37584,7 +37577,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" s="37" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B173" s="37" t="s">
         <v>331</v>
@@ -37596,7 +37589,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" s="37" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B174" s="37" t="s">
         <v>331</v>
@@ -37608,7 +37601,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" s="37" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B175" s="37" t="s">
         <v>331</v>
@@ -37620,7 +37613,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" s="37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B176" s="37" t="s">
         <v>331</v>
@@ -37632,7 +37625,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" s="37" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B177" s="37" t="s">
         <v>331</v>
@@ -37644,7 +37637,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" s="37" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B178" s="37" t="s">
         <v>331</v>
@@ -37656,7 +37649,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" s="37" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B179" s="37" t="s">
         <v>331</v>
@@ -37668,7 +37661,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" s="37" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B180" s="37" t="s">
         <v>331</v>
@@ -37680,7 +37673,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B181" s="37" t="s">
         <v>331</v>
@@ -37692,7 +37685,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" s="37" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B182" s="37" t="s">
         <v>331</v>
@@ -37704,7 +37697,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A183" s="37" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B183" s="37" t="s">
         <v>331</v>
@@ -37716,7 +37709,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A184" s="37" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B184" s="37" t="s">
         <v>331</v>
@@ -37728,7 +37721,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" s="37" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B185" s="37" t="s">
         <v>331</v>
@@ -37740,7 +37733,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" s="37" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B186" s="37" t="s">
         <v>331</v>
@@ -37752,7 +37745,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" s="37" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B187" s="37" t="s">
         <v>331</v>
@@ -37764,7 +37757,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A188" s="37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B188" s="37" t="s">
         <v>331</v>
@@ -37776,7 +37769,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" s="37" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B189" s="37" t="s">
         <v>331</v>
@@ -37788,7 +37781,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" s="37" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B190" s="37" t="s">
         <v>331</v>
@@ -37800,7 +37793,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" s="37" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B191" s="37" t="s">
         <v>331</v>
@@ -37812,7 +37805,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" s="37" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B192" s="37" t="s">
         <v>331</v>
@@ -37824,7 +37817,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" s="37" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B193" s="37" t="s">
         <v>331</v>
@@ -37836,7 +37829,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" s="37" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B194" s="37" t="s">
         <v>331</v>
@@ -37848,7 +37841,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B195" s="37" t="s">
         <v>331</v>
@@ -37860,7 +37853,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" s="37" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B196" s="37" t="s">
         <v>331</v>
@@ -37872,7 +37865,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A197" s="37" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B197" s="37" t="s">
         <v>331</v>
@@ -37884,7 +37877,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A198" s="37" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B198" s="37" t="s">
         <v>331</v>
@@ -37896,7 +37889,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" s="37" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B199" s="37" t="s">
         <v>331</v>
@@ -37908,7 +37901,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" s="37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B200" s="37" t="s">
         <v>331</v>
@@ -37920,7 +37913,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" s="37" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B201" s="37" t="s">
         <v>331</v>
@@ -37932,7 +37925,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" s="37" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B202" s="37" t="s">
         <v>331</v>
@@ -37944,7 +37937,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" s="37" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B203" s="37" t="s">
         <v>331</v>
@@ -37956,7 +37949,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" s="37" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B204" s="37" t="s">
         <v>331</v>
@@ -37968,7 +37961,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" s="37" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B205" s="37" t="s">
         <v>331</v>
@@ -37980,7 +37973,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" s="37" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B206" s="37" t="s">
         <v>331</v>
@@ -37992,7 +37985,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" s="37" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B207" s="37" t="s">
         <v>331</v>
@@ -38004,7 +37997,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" s="37" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B208" s="37" t="s">
         <v>331</v>
@@ -38016,7 +38009,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" s="37" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B209" s="37" t="s">
         <v>331</v>
@@ -38028,7 +38021,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" s="37" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B210" s="37" t="s">
         <v>331</v>
@@ -38040,7 +38033,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" s="37" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B211" s="37" t="s">
         <v>331</v>
@@ -38052,7 +38045,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" s="37" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B212" s="37" t="s">
         <v>331</v>
@@ -38064,7 +38057,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" s="37" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B213" s="37" t="s">
         <v>331</v>
@@ -38076,7 +38069,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" s="37" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B214" s="37" t="s">
         <v>331</v>
@@ -38088,7 +38081,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" s="37" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B215" s="37" t="s">
         <v>331</v>
@@ -38100,7 +38093,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" s="37" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B216" s="37" t="s">
         <v>331</v>
@@ -38112,7 +38105,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" s="37" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B217" s="37" t="s">
         <v>331</v>
@@ -38124,7 +38117,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" s="37" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B218" s="37" t="s">
         <v>331</v>
@@ -38136,7 +38129,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A219" s="37" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B219" s="37" t="s">
         <v>331</v>
@@ -38148,7 +38141,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A220" s="37" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B220" s="37" t="s">
         <v>331</v>
@@ -38160,7 +38153,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A221" s="37" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B221" s="37" t="s">
         <v>331</v>
@@ -38172,7 +38165,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A222" s="37" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B222" s="37" t="s">
         <v>331</v>
@@ -38184,7 +38177,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A223" s="37" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B223" s="37" t="s">
         <v>331</v>
@@ -38196,7 +38189,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A224" s="37" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B224" s="37" t="s">
         <v>331</v>
@@ -38208,7 +38201,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A225" s="37" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B225" s="37" t="s">
         <v>331</v>
@@ -38220,7 +38213,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A226" s="37" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B226" s="37" t="s">
         <v>331</v>
@@ -38232,7 +38225,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A227" s="37" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B227" s="37" t="s">
         <v>331</v>
@@ -38244,7 +38237,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A228" s="37" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B228" s="37" t="s">
         <v>331</v>
@@ -38256,7 +38249,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A229" s="37" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B229" s="37" t="s">
         <v>331</v>
@@ -38268,7 +38261,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A230" s="37" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B230" s="37" t="s">
         <v>331</v>
@@ -38280,7 +38273,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A231" s="37" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B231" s="37" t="s">
         <v>331</v>
@@ -38292,7 +38285,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A232" s="37" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B232" s="37" t="s">
         <v>331</v>
@@ -38304,7 +38297,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A233" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B233" s="37" t="s">
         <v>331</v>
@@ -38316,7 +38309,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A234" s="37" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B234" s="37" t="s">
         <v>331</v>
@@ -38328,7 +38321,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A235" s="37" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B235" s="37" t="s">
         <v>331</v>
@@ -38340,7 +38333,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A236" s="37" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B236" s="37" t="s">
         <v>331</v>
@@ -38352,7 +38345,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A237" s="37" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B237" s="37" t="s">
         <v>331</v>
@@ -38364,7 +38357,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A238" s="37" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B238" s="37" t="s">
         <v>331</v>
@@ -38376,7 +38369,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A239" s="37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B239" s="37" t="s">
         <v>331</v>
@@ -38388,7 +38381,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A240" s="37" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B240" s="37" t="s">
         <v>331</v>
@@ -38400,7 +38393,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A241" s="37" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B241" s="37" t="s">
         <v>331</v>
@@ -38412,7 +38405,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A242" s="37" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B242" s="37" t="s">
         <v>331</v>
@@ -38424,7 +38417,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A243" s="37" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B243" s="37" t="s">
         <v>331</v>
@@ -38436,7 +38429,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A244" s="37" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B244" s="37" t="s">
         <v>331</v>
@@ -38448,7 +38441,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A245" s="37" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B245" s="37" t="s">
         <v>331</v>
@@ -38460,7 +38453,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A246" s="37" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B246" s="37" t="s">
         <v>331</v>
@@ -38472,7 +38465,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A247" s="37" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B247" s="37" t="s">
         <v>331</v>
@@ -38484,7 +38477,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B248" s="37" t="s">
         <v>331</v>
@@ -38496,7 +38489,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" s="37" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B249" s="37" t="s">
         <v>331</v>
@@ -38508,7 +38501,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" s="37" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B250" s="37" t="s">
         <v>331</v>
@@ -38520,7 +38513,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" s="37" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B251" s="37" t="s">
         <v>331</v>
@@ -38532,7 +38525,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" s="37" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B252" s="37" t="s">
         <v>331</v>
@@ -38544,7 +38537,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A253" s="37" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B253" s="37" t="s">
         <v>331</v>
@@ -38556,7 +38549,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A254" s="37" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B254" s="37" t="s">
         <v>331</v>
@@ -38568,7 +38561,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" s="37" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B255" s="37" t="s">
         <v>331</v>
@@ -38580,7 +38573,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" s="37" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B256" s="37" t="s">
         <v>331</v>
@@ -38592,7 +38585,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A257" s="37" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B257" s="37" t="s">
         <v>331</v>
@@ -38604,7 +38597,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A258" s="37" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B258" s="37" t="s">
         <v>331</v>
@@ -38616,7 +38609,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A259" s="37" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B259" s="37" t="s">
         <v>331</v>
@@ -38628,7 +38621,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A260" s="37" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B260" s="37" t="s">
         <v>331</v>
@@ -38640,7 +38633,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A261" s="37" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B261" s="37" t="s">
         <v>331</v>
@@ -38652,7 +38645,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A262" s="37" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B262" s="37" t="s">
         <v>331</v>
@@ -38664,7 +38657,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A263" s="37" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B263" s="37" t="s">
         <v>331</v>
@@ -38676,7 +38669,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A264" s="37" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B264" s="37" t="s">
         <v>331</v>
@@ -38688,7 +38681,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A265" s="37" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B265" s="37" t="s">
         <v>331</v>
@@ -38700,7 +38693,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A266" s="37" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B266" s="37" t="s">
         <v>331</v>
@@ -38712,7 +38705,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A267" s="37" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B267" s="37" t="s">
         <v>331</v>
@@ -38724,7 +38717,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A268" s="37" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B268" s="37" t="s">
         <v>331</v>
@@ -38736,7 +38729,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" s="37" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B269" s="37" t="s">
         <v>331</v>
@@ -38748,7 +38741,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" s="37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B270" s="37" t="s">
         <v>331</v>
@@ -38760,7 +38753,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A271" s="37" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B271" s="37" t="s">
         <v>331</v>
@@ -38772,7 +38765,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A272" s="37" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B272" s="37" t="s">
         <v>331</v>
@@ -38784,7 +38777,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" s="37" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B273" s="37" t="s">
         <v>331</v>
@@ -38796,7 +38789,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" s="37" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B274" s="37" t="s">
         <v>331</v>
@@ -38808,7 +38801,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" s="37" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B275" s="37" t="s">
         <v>331</v>
@@ -38820,7 +38813,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" s="37" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B276" s="37" t="s">
         <v>331</v>
@@ -38832,7 +38825,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A277" s="37" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B277" s="37" t="s">
         <v>331</v>
@@ -38844,7 +38837,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" s="37" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B278" s="37" t="s">
         <v>331</v>
@@ -38856,7 +38849,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B279" s="37" t="s">
         <v>331</v>
@@ -38868,7 +38861,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" s="37" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B280" s="37" t="s">
         <v>331</v>
@@ -38880,7 +38873,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" s="37" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B281" s="37" t="s">
         <v>331</v>
@@ -38892,7 +38885,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" s="37" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B282" s="37" t="s">
         <v>331</v>
@@ -38904,7 +38897,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" s="37" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B283" s="37" t="s">
         <v>331</v>
@@ -38916,7 +38909,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" s="37" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B284" s="37" t="s">
         <v>331</v>
@@ -38928,7 +38921,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" s="37" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B285" s="37" t="s">
         <v>331</v>
@@ -38940,7 +38933,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" s="37" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B286" s="37" t="s">
         <v>331</v>
@@ -38952,7 +38945,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" s="37" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B287" s="37" t="s">
         <v>331</v>
@@ -38964,7 +38957,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" s="37" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B288" s="37" t="s">
         <v>331</v>
@@ -38976,7 +38969,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" s="37" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B289" s="37" t="s">
         <v>331</v>
@@ -38988,7 +38981,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" s="37" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B290" s="37" t="s">
         <v>331</v>
@@ -39000,7 +38993,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" s="37" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B291" s="37" t="s">
         <v>331</v>
@@ -39012,7 +39005,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" s="37" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B292" s="37" t="s">
         <v>331</v>
@@ -39024,7 +39017,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" s="37" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B293" s="37" t="s">
         <v>331</v>
@@ -39036,7 +39029,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" s="37" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B294" s="37" t="s">
         <v>331</v>
@@ -39048,7 +39041,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" s="37" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B295" s="37" t="s">
         <v>331</v>
@@ -39060,7 +39053,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" s="37" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B296" s="37" t="s">
         <v>331</v>
@@ -39072,7 +39065,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A297" s="37" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B297" s="37" t="s">
         <v>331</v>
@@ -39084,7 +39077,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A298" s="37" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B298" s="37" t="s">
         <v>331</v>
@@ -39096,7 +39089,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" s="37" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B299" s="37" t="s">
         <v>331</v>
@@ -39108,7 +39101,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" s="37" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B300" s="37" t="s">
         <v>331</v>
@@ -39120,7 +39113,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" s="37" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B301" s="37" t="s">
         <v>331</v>
@@ -39132,7 +39125,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" s="37" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B302" s="37" t="s">
         <v>331</v>
@@ -39144,7 +39137,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A303" s="37" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B303" s="37" t="s">
         <v>331</v>
@@ -39156,7 +39149,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A304" s="37" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B304" s="37" t="s">
         <v>331</v>
@@ -39168,7 +39161,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" s="37" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B305" s="37" t="s">
         <v>331</v>
@@ -39180,7 +39173,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B306" s="37" t="s">
         <v>331</v>
@@ -39192,7 +39185,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" s="37" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B307" s="37" t="s">
         <v>331</v>
@@ -39204,7 +39197,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A308" s="37" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B308" s="37" t="s">
         <v>331</v>
@@ -39216,7 +39209,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A309" s="37" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B309" s="37" t="s">
         <v>331</v>
@@ -39228,7 +39221,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" s="37" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B310" s="37" t="s">
         <v>331</v>
@@ -39240,7 +39233,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" s="37" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B311" s="37" t="s">
         <v>331</v>
@@ -39252,7 +39245,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" s="37" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B312" s="37" t="s">
         <v>331</v>
@@ -39264,7 +39257,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" s="37" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B313" s="37" t="s">
         <v>331</v>
@@ -39276,7 +39269,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" s="37" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B314" s="37" t="s">
         <v>331</v>
@@ -39288,7 +39281,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" s="37" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B315" s="37" t="s">
         <v>331</v>
@@ -39300,7 +39293,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" s="37" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B316" s="37" t="s">
         <v>331</v>
@@ -39312,7 +39305,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" s="37" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B317" s="37" t="s">
         <v>331</v>
@@ -39324,7 +39317,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" s="37" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B318" s="37" t="s">
         <v>331</v>
@@ -39336,7 +39329,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="37" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B319" s="37" t="s">
         <v>331</v>
@@ -39348,7 +39341,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A320" s="37" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B320" s="37" t="s">
         <v>331</v>
@@ -39360,7 +39353,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A321" s="37" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B321" s="37" t="s">
         <v>331</v>
@@ -39372,7 +39365,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" s="37" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B322" s="37" t="s">
         <v>331</v>
@@ -39384,7 +39377,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A323" s="37" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B323" s="37" t="s">
         <v>331</v>
@@ -39396,7 +39389,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A324" s="37" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B324" s="37" t="s">
         <v>331</v>
@@ -39408,7 +39401,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B325" s="37" t="s">
         <v>331</v>
@@ -39420,7 +39413,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" s="37" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B326" s="37" t="s">
         <v>331</v>
@@ -39432,7 +39425,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" s="37" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B327" s="37" t="s">
         <v>331</v>
@@ -39444,7 +39437,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" s="37" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B328" s="37" t="s">
         <v>331</v>
@@ -39456,7 +39449,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" s="37" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B329" s="37" t="s">
         <v>331</v>
@@ -39468,7 +39461,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" s="37" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B330" s="37" t="s">
         <v>331</v>
@@ -39480,7 +39473,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" s="37" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B331" s="37" t="s">
         <v>331</v>
@@ -39492,7 +39485,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" s="37" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B332" s="37" t="s">
         <v>331</v>
@@ -39504,7 +39497,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" s="37" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B333" s="37" t="s">
         <v>331</v>
@@ -39516,7 +39509,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A334" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B334" s="37" t="s">
         <v>331</v>
@@ -39528,7 +39521,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A335" s="37" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B335" s="37" t="s">
         <v>331</v>
@@ -39540,7 +39533,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" s="37" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B336" s="37" t="s">
         <v>331</v>
@@ -39552,7 +39545,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" s="37" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B337" s="37" t="s">
         <v>331</v>
@@ -39564,7 +39557,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A338" s="37" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B338" s="37" t="s">
         <v>331</v>
@@ -39576,7 +39569,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" s="37" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B339" s="37" t="s">
         <v>331</v>
@@ -39588,7 +39581,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" s="37" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B340" s="37" t="s">
         <v>331</v>
@@ -39600,7 +39593,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" s="37" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B341" s="37" t="s">
         <v>331</v>
@@ -39612,7 +39605,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" s="37" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B342" s="37" t="s">
         <v>331</v>
@@ -39624,7 +39617,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" s="37" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B343" s="37" t="s">
         <v>331</v>
@@ -39636,7 +39629,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" s="37" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B344" s="37" t="s">
         <v>331</v>
@@ -39648,7 +39641,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A345" s="37" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B345" s="37" t="s">
         <v>331</v>
@@ -39660,7 +39653,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A346" s="37" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B346" s="37" t="s">
         <v>331</v>
@@ -39672,7 +39665,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" s="37" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B347" s="37" t="s">
         <v>331</v>
@@ -39684,7 +39677,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A348" s="37" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B348" s="37" t="s">
         <v>331</v>
@@ -39696,7 +39689,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A349" s="37" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B349" s="37" t="s">
         <v>331</v>
@@ -39708,7 +39701,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A350" s="37" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B350" s="37" t="s">
         <v>331</v>
@@ -39720,7 +39713,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" s="37" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B351" s="37" t="s">
         <v>331</v>
@@ -39732,7 +39725,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A352" s="37" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B352" s="37" t="s">
         <v>331</v>
@@ -39744,7 +39737,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A353" s="37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B353" s="37" t="s">
         <v>331</v>
@@ -39756,7 +39749,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A354" s="37" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B354" s="37" t="s">
         <v>331</v>
@@ -39768,7 +39761,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A355" s="37" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B355" s="37" t="s">
         <v>331</v>
@@ -39780,7 +39773,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A356" s="37" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B356" s="37" t="s">
         <v>331</v>
@@ -39792,7 +39785,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A357" s="37" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B357" s="37" t="s">
         <v>331</v>
@@ -39804,7 +39797,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A358" s="37" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B358" s="37" t="s">
         <v>331</v>
@@ -39816,7 +39809,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A359" s="37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B359" s="37" t="s">
         <v>331</v>
@@ -39828,7 +39821,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A360" s="37" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B360" s="37" t="s">
         <v>331</v>
@@ -39840,7 +39833,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A361" s="37" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B361" s="37" t="s">
         <v>331</v>
@@ -39852,7 +39845,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A362" s="37" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B362" s="37" t="s">
         <v>331</v>
@@ -39864,7 +39857,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A363" s="37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B363" s="37" t="s">
         <v>331</v>
@@ -39876,7 +39869,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A364" s="37" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B364" s="37" t="s">
         <v>331</v>
@@ -39888,7 +39881,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A365" s="37" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B365" s="37" t="s">
         <v>331</v>
@@ -39900,7 +39893,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A366" s="37" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B366" s="37" t="s">
         <v>331</v>
@@ -39912,7 +39905,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A367" s="37" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B367" s="37" t="s">
         <v>331</v>
@@ -39924,7 +39917,7 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A368" s="37" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B368" s="37" t="s">
         <v>331</v>
@@ -39936,7 +39929,7 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A369" s="37" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B369" s="37" t="s">
         <v>331</v>
@@ -39948,7 +39941,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A370" s="37" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B370" s="37" t="s">
         <v>331</v>
@@ -39960,7 +39953,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A371" s="37" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B371" s="37" t="s">
         <v>331</v>
@@ -39972,7 +39965,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A372" s="37" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B372" s="37" t="s">
         <v>331</v>
@@ -39984,7 +39977,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A373" s="37" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B373" s="37" t="s">
         <v>331</v>
@@ -39996,7 +39989,7 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A374" s="37" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B374" s="37" t="s">
         <v>331</v>
@@ -40008,7 +40001,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A375" s="37" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B375" s="37" t="s">
         <v>331</v>
@@ -40020,7 +40013,7 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A376" s="37" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B376" s="37" t="s">
         <v>331</v>
@@ -40032,7 +40025,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A377" s="37" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B377" s="37" t="s">
         <v>331</v>
@@ -40044,7 +40037,7 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A378" s="37" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B378" s="37" t="s">
         <v>331</v>
@@ -40056,7 +40049,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A379" s="37" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B379" s="37" t="s">
         <v>331</v>
@@ -40068,7 +40061,7 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A380" s="37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B380" s="37" t="s">
         <v>331</v>
@@ -40080,7 +40073,7 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A381" s="37" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B381" s="37" t="s">
         <v>331</v>
@@ -40092,7 +40085,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A382" s="37" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B382" s="37" t="s">
         <v>331</v>
@@ -40104,7 +40097,7 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A383" s="37" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B383" s="37" t="s">
         <v>331</v>
@@ -40116,7 +40109,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A384" s="37" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B384" s="37" t="s">
         <v>331</v>
@@ -40128,7 +40121,7 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A385" s="37" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B385" s="37" t="s">
         <v>331</v>
@@ -40140,7 +40133,7 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A386" s="37" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B386" s="37" t="s">
         <v>331</v>
@@ -40152,7 +40145,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A387" s="37" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B387" s="37" t="s">
         <v>331</v>
@@ -40164,7 +40157,7 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A388" s="37" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B388" s="37" t="s">
         <v>331</v>
@@ -40176,7 +40169,7 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A389" s="37" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B389" s="37" t="s">
         <v>331</v>
@@ -40188,7 +40181,7 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A390" s="37" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B390" s="37" t="s">
         <v>331</v>
@@ -40200,7 +40193,7 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A391" s="37" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B391" s="37" t="s">
         <v>331</v>
@@ -40212,7 +40205,7 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A392" s="37" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B392" s="37" t="s">
         <v>331</v>
@@ -40224,7 +40217,7 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A393" s="37" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B393" s="37" t="s">
         <v>331</v>
@@ -40236,7 +40229,7 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A394" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B394" s="37" t="s">
         <v>331</v>
@@ -40248,7 +40241,7 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A395" s="37" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B395" s="37" t="s">
         <v>331</v>
@@ -40260,7 +40253,7 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A396" s="37" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B396" s="37" t="s">
         <v>331</v>
@@ -40272,7 +40265,7 @@
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A397" s="37" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B397" s="37" t="s">
         <v>331</v>
@@ -40284,7 +40277,7 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A398" s="37" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B398" s="37" t="s">
         <v>331</v>
@@ -40296,7 +40289,7 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A399" s="37" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B399" s="37" t="s">
         <v>331</v>
@@ -40308,7 +40301,7 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A400" s="37" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B400" s="37" t="s">
         <v>331</v>
@@ -40320,7 +40313,7 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A401" s="37" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B401" s="37" t="s">
         <v>331</v>
@@ -40332,7 +40325,7 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A402" s="37" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B402" s="37" t="s">
         <v>331</v>
@@ -40344,7 +40337,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A403" s="37" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B403" s="37" t="s">
         <v>331</v>
@@ -40356,7 +40349,7 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A404" s="37" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B404" s="37" t="s">
         <v>331</v>
@@ -40368,7 +40361,7 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A405" s="37" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B405" s="37" t="s">
         <v>331</v>
@@ -40380,7 +40373,7 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A406" s="37" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B406" s="37" t="s">
         <v>331</v>
@@ -40392,7 +40385,7 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A407" s="37" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B407" s="37" t="s">
         <v>331</v>
@@ -40404,7 +40397,7 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A408" s="37" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B408" s="37" t="s">
         <v>331</v>
@@ -40416,7 +40409,7 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A409" s="37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B409" s="37" t="s">
         <v>331</v>
@@ -40428,7 +40421,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A410" s="37" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B410" s="37" t="s">
         <v>331</v>
@@ -40440,7 +40433,7 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A411" s="37" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B411" s="37" t="s">
         <v>331</v>
@@ -40452,7 +40445,7 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A412" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B412" s="37" t="s">
         <v>331</v>
@@ -40464,7 +40457,7 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A413" s="37" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B413" s="37" t="s">
         <v>331</v>
@@ -40476,7 +40469,7 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A414" s="37" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B414" s="37" t="s">
         <v>331</v>
@@ -40488,7 +40481,7 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A415" s="37" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B415" s="37" t="s">
         <v>331</v>
@@ -40500,7 +40493,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A416" s="37" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B416" s="37" t="s">
         <v>331</v>
@@ -40512,7 +40505,7 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A417" s="37" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B417" s="37" t="s">
         <v>331</v>
@@ -40524,7 +40517,7 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A418" s="37" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B418" s="37" t="s">
         <v>331</v>
@@ -40536,7 +40529,7 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A419" s="37" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B419" s="37" t="s">
         <v>331</v>
@@ -40548,7 +40541,7 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A420" s="37" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B420" s="37" t="s">
         <v>331</v>
@@ -40560,7 +40553,7 @@
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A421" s="37" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B421" s="37" t="s">
         <v>331</v>
@@ -40572,7 +40565,7 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A422" s="37" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B422" s="37" t="s">
         <v>331</v>
@@ -40584,7 +40577,7 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A423" s="37" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B423" s="37" t="s">
         <v>331</v>
@@ -40596,7 +40589,7 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A424" s="37" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B424" s="37" t="s">
         <v>331</v>
@@ -40608,7 +40601,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A425" s="37" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B425" s="37" t="s">
         <v>331</v>
@@ -40620,7 +40613,7 @@
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A426" s="37" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B426" s="37" t="s">
         <v>331</v>
@@ -40632,7 +40625,7 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A427" s="37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B427" s="37" t="s">
         <v>331</v>
@@ -40644,7 +40637,7 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A428" s="37" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B428" s="37" t="s">
         <v>331</v>
@@ -40656,7 +40649,7 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A429" s="37" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B429" s="37" t="s">
         <v>331</v>
@@ -40668,7 +40661,7 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A430" s="37" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B430" s="37" t="s">
         <v>331</v>
@@ -40680,7 +40673,7 @@
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A431" s="37" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B431" s="37" t="s">
         <v>331</v>
@@ -40692,7 +40685,7 @@
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A432" s="37" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B432" s="37" t="s">
         <v>331</v>
@@ -40704,7 +40697,7 @@
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A433" s="37" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B433" s="37" t="s">
         <v>331</v>
@@ -40716,7 +40709,7 @@
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A434" s="37" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B434" s="37" t="s">
         <v>331</v>
@@ -40728,7 +40721,7 @@
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A435" s="37" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B435" s="37" t="s">
         <v>331</v>
@@ -40740,7 +40733,7 @@
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A436" s="37" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B436" s="37" t="s">
         <v>331</v>
@@ -40752,7 +40745,7 @@
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A437" s="37" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B437" s="37" t="s">
         <v>331</v>
@@ -40764,7 +40757,7 @@
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A438" s="37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B438" s="37" t="s">
         <v>331</v>
@@ -40776,7 +40769,7 @@
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A439" s="37" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B439" s="37" t="s">
         <v>331</v>
@@ -40788,7 +40781,7 @@
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A440" s="37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B440" s="37" t="s">
         <v>331</v>
@@ -40800,7 +40793,7 @@
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A441" s="37" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B441" s="37" t="s">
         <v>331</v>
@@ -40812,7 +40805,7 @@
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A442" s="37" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B442" s="37" t="s">
         <v>331</v>
@@ -40824,7 +40817,7 @@
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A443" s="37" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B443" s="37" t="s">
         <v>331</v>
@@ -40836,7 +40829,7 @@
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A444" s="37" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B444" s="37" t="s">
         <v>331</v>
@@ -40848,7 +40841,7 @@
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A445" s="37" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B445" s="37" t="s">
         <v>331</v>
@@ -40860,7 +40853,7 @@
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A446" s="37" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B446" s="37" t="s">
         <v>331</v>
@@ -40872,7 +40865,7 @@
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A447" s="37" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B447" s="37" t="s">
         <v>331</v>
@@ -40884,7 +40877,7 @@
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A448" s="37" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B448" s="37" t="s">
         <v>331</v>
@@ -40896,7 +40889,7 @@
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A449" s="37" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B449" s="37" t="s">
         <v>331</v>
@@ -40908,7 +40901,7 @@
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A450" s="37" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B450" s="37" t="s">
         <v>331</v>
@@ -40920,7 +40913,7 @@
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A451" s="37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B451" s="37" t="s">
         <v>331</v>
@@ -40932,7 +40925,7 @@
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A452" s="37" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B452" s="37" t="s">
         <v>331</v>
@@ -40944,7 +40937,7 @@
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A453" s="37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B453" s="37" t="s">
         <v>331</v>
@@ -40956,7 +40949,7 @@
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A454" s="37" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B454" s="37" t="s">
         <v>331</v>
@@ -40968,7 +40961,7 @@
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A455" s="37" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B455" s="37" t="s">
         <v>331</v>
@@ -40980,7 +40973,7 @@
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A456" s="37" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B456" s="37" t="s">
         <v>331</v>
@@ -40992,7 +40985,7 @@
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A457" s="37" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B457" s="37" t="s">
         <v>331</v>
@@ -41004,7 +40997,7 @@
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A458" s="37" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B458" s="37" t="s">
         <v>331</v>
@@ -41016,7 +41009,7 @@
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A459" s="37" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B459" s="37" t="s">
         <v>331</v>
@@ -41028,7 +41021,7 @@
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A460" s="37" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B460" s="37" t="s">
         <v>331</v>
@@ -41040,7 +41033,7 @@
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A461" s="37" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B461" s="37" t="s">
         <v>331</v>
@@ -41052,7 +41045,7 @@
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A462" s="37" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B462" s="37" t="s">
         <v>331</v>
@@ -41064,7 +41057,7 @@
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A463" s="37" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B463" s="37" t="s">
         <v>331</v>
@@ -41076,7 +41069,7 @@
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A464" s="37" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B464" s="37" t="s">
         <v>331</v>
@@ -41088,7 +41081,7 @@
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A465" s="37" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B465" s="37" t="s">
         <v>331</v>
@@ -41100,7 +41093,7 @@
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A466" s="37" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B466" s="37" t="s">
         <v>331</v>
@@ -41112,7 +41105,7 @@
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A467" s="37" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B467" s="37" t="s">
         <v>331</v>
@@ -41124,7 +41117,7 @@
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A468" s="37" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B468" s="37" t="s">
         <v>331</v>
@@ -41136,7 +41129,7 @@
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A469" s="37" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B469" s="37" t="s">
         <v>331</v>
@@ -41148,7 +41141,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A470" s="37" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B470" s="37" t="s">
         <v>331</v>
@@ -41160,7 +41153,7 @@
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A471" s="37" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B471" s="37" t="s">
         <v>331</v>
@@ -41172,7 +41165,7 @@
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A472" s="37" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B472" s="37" t="s">
         <v>331</v>
@@ -41184,7 +41177,7 @@
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A473" s="37" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B473" s="37" t="s">
         <v>331</v>
@@ -41196,7 +41189,7 @@
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A474" s="37" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B474" s="37" t="s">
         <v>331</v>
@@ -41208,7 +41201,7 @@
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A475" s="37" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B475" s="37" t="s">
         <v>331</v>
@@ -41220,7 +41213,7 @@
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A476" s="37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B476" s="37" t="s">
         <v>331</v>
@@ -41232,7 +41225,7 @@
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A477" s="37" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B477" s="37" t="s">
         <v>331</v>
@@ -41244,7 +41237,7 @@
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A478" s="34" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B478" s="37" t="s">
         <v>331</v>
@@ -41256,7 +41249,7 @@
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A479" s="34" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B479" s="37" t="s">
         <v>331</v>
@@ -41268,7 +41261,7 @@
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A480" s="34" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B480" s="37" t="s">
         <v>331</v>
@@ -41280,7 +41273,7 @@
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A481" s="34" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B481" s="37" t="s">
         <v>331</v>
@@ -41292,7 +41285,7 @@
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A482" s="34" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B482" s="37" t="s">
         <v>331</v>
@@ -41304,7 +41297,7 @@
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A483" s="34" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B483" s="37" t="s">
         <v>331</v>
@@ -41316,7 +41309,7 @@
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A484" s="34" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B484" s="37" t="s">
         <v>331</v>
@@ -41328,7 +41321,7 @@
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A485" s="34" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B485" s="37" t="s">
         <v>331</v>
@@ -41340,7 +41333,7 @@
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A486" s="37" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B486" s="37" t="s">
         <v>331</v>
@@ -41352,7 +41345,7 @@
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A487" s="37" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B487" s="37" t="s">
         <v>331</v>
@@ -41364,7 +41357,7 @@
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A488" s="37" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B488" s="37" t="s">
         <v>331</v>
@@ -41376,7 +41369,7 @@
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A489" s="37" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B489" s="37" t="s">
         <v>331</v>
@@ -41388,7 +41381,7 @@
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A490" s="37" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B490" s="37" t="s">
         <v>331</v>
@@ -41400,7 +41393,7 @@
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A491" s="37" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B491" s="37" t="s">
         <v>331</v>
@@ -41412,7 +41405,7 @@
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A492" s="37" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B492" s="37" t="s">
         <v>331</v>
@@ -41424,7 +41417,7 @@
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A493" s="37" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B493" s="37" t="s">
         <v>331</v>
@@ -41436,7 +41429,7 @@
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A494" s="37" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B494" s="37" t="s">
         <v>331</v>
@@ -41448,7 +41441,7 @@
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A495" s="37" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B495" s="37" t="s">
         <v>331</v>
@@ -41460,7 +41453,7 @@
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A496" s="37" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B496" s="37" t="s">
         <v>331</v>
@@ -41472,7 +41465,7 @@
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A497" s="37" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B497" s="37" t="s">
         <v>331</v>
@@ -41484,7 +41477,7 @@
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A498" s="37" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B498" s="37" t="s">
         <v>331</v>

</xml_diff>